<commit_message>
Added Youtuber email addresses
</commit_message>
<xml_diff>
--- a/Marketing planning.xlsx
+++ b/Marketing planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wstoop\Documents\thesapling-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAED22BE-E184-4A86-AC8F-E4FED5122ECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F227DBF-B957-4AF4-B86B-6752F953AEFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" activeTab="6" xr2:uid="{F29F535E-B8F5-49A6-BD0B-95E582B571D1}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="501">
   <si>
     <t>Week</t>
   </si>
@@ -1532,6 +1532,24 @@
   </si>
   <si>
     <t>manyatruenerd@gmail.com</t>
+  </si>
+  <si>
+    <t>predaindex@gmail.com</t>
+  </si>
+  <si>
+    <t>elescocesgamer@gmail.com</t>
+  </si>
+  <si>
+    <t>DieselDesignsGaming@gmail.com</t>
+  </si>
+  <si>
+    <t>Zach</t>
+  </si>
+  <si>
+    <t>spanglzj@gmail.com</t>
+  </si>
+  <si>
+    <t>cheru2016yt@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2911,10 +2929,10 @@
   <dimension ref="A1:P310"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M19" sqref="M19"/>
+      <selection pane="bottomRight" activeCell="N116" sqref="N59:N116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3859,7 +3877,7 @@
         <v>38</v>
       </c>
       <c r="N60" t="s">
-        <v>463</v>
+        <v>495</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
@@ -4315,7 +4333,7 @@
         <v>9</v>
       </c>
       <c r="N94" t="s">
-        <v>463</v>
+        <v>500</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.3">
@@ -4372,7 +4390,7 @@
         <v>17</v>
       </c>
       <c r="N98" t="s">
-        <v>463</v>
+        <v>496</v>
       </c>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
@@ -4546,7 +4564,7 @@
         <v>4.5</v>
       </c>
       <c r="N111" t="s">
-        <v>463</v>
+        <v>497</v>
       </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.3">
@@ -4612,7 +4630,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="N116" t="s">
-        <v>463</v>
+        <v>499</v>
+      </c>
+      <c r="O116" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added more email addresses
</commit_message>
<xml_diff>
--- a/Marketing planning.xlsx
+++ b/Marketing planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wstoop\Documents\thesapling-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E52DA5-EB25-4201-9E06-D1D1DC99F835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E80E06-8010-405C-BA85-FB7AA3FFCEE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" firstSheet="2" activeTab="6" xr2:uid="{F29F535E-B8F5-49A6-BD0B-95E582B571D1}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="731">
   <si>
     <t>Week</t>
   </si>
@@ -2016,12 +2016,258 @@
   <si>
     <t>modioperandus@gmail.com</t>
   </si>
+  <si>
+    <t>dzaran</t>
+  </si>
+  <si>
+    <t>Aavak</t>
+  </si>
+  <si>
+    <t>aavak@snowspider.com</t>
+  </si>
+  <si>
+    <t>Muzzloff</t>
+  </si>
+  <si>
+    <t>avmuzlov@gmail.com</t>
+  </si>
+  <si>
+    <t>フルツチ - HuLtuTi</t>
+  </si>
+  <si>
+    <t>hultutitv@gmail.com</t>
+  </si>
+  <si>
+    <t>OfficialNerdCubed</t>
+  </si>
+  <si>
+    <t>business@nerdcubed.co.uk</t>
+  </si>
+  <si>
+    <t>KatherineOfSky</t>
+  </si>
+  <si>
+    <t>katherineofsky@gmail.com</t>
+  </si>
+  <si>
+    <t>DSimphony</t>
+  </si>
+  <si>
+    <t>contacto@dsimphony.com</t>
+  </si>
+  <si>
+    <t>Fynnpire</t>
+  </si>
+  <si>
+    <t>fynnpire@gmail.com</t>
+  </si>
+  <si>
+    <t>JoePad17</t>
+  </si>
+  <si>
+    <t>jpad17officialchannel@gmail.com</t>
+  </si>
+  <si>
+    <t>Krekerman</t>
+  </si>
+  <si>
+    <t>Ctop</t>
+  </si>
+  <si>
+    <t>Ctop@screenwavemedia.com</t>
+  </si>
+  <si>
+    <t>DraaxLP</t>
+  </si>
+  <si>
+    <t>draax@draaxlp.com</t>
+  </si>
+  <si>
+    <t>mischa gaming</t>
+  </si>
+  <si>
+    <t>Mischa</t>
+  </si>
+  <si>
+    <t>mischacrossing@gmail.com</t>
+  </si>
+  <si>
+    <t>Erakol</t>
+  </si>
+  <si>
+    <t>erakol.ger@gmail.com</t>
+  </si>
+  <si>
+    <t>NestafeLP</t>
+  </si>
+  <si>
+    <t>gaminggoeren@gmail.com</t>
+  </si>
+  <si>
+    <t>TinyPirate</t>
+  </si>
+  <si>
+    <t>peter@tinypirate.com</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Sir Taptap</t>
+  </si>
+  <si>
+    <t>Contact@sirtaptap.com</t>
+  </si>
+  <si>
+    <t>Delphron</t>
+  </si>
+  <si>
+    <t>nigelfitz20@gmail.com</t>
+  </si>
+  <si>
+    <t>Reyson</t>
+  </si>
+  <si>
+    <t>reysonfr@gmail.com</t>
+  </si>
+  <si>
+    <t>Pinkfate</t>
+  </si>
+  <si>
+    <t>pinkfategamesyt@gmail.com</t>
+  </si>
+  <si>
+    <t>I Febag</t>
+  </si>
+  <si>
+    <t>FebagTeam@gmail.com</t>
+  </si>
+  <si>
+    <t>MishiaruFR</t>
+  </si>
+  <si>
+    <t>Maxdaling@gmail.com</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>GameFace</t>
+  </si>
+  <si>
+    <t>Kateriix</t>
+  </si>
+  <si>
+    <t>te weinig views nieuwe videos</t>
+  </si>
+  <si>
+    <t>BaronVonGames</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baronvonbusiness@gmail.com </t>
+  </si>
+  <si>
+    <t>info@contranetwork.it</t>
+  </si>
+  <si>
+    <t>ContraNetwork</t>
+  </si>
+  <si>
+    <t>Kindly Keyin</t>
+  </si>
+  <si>
+    <t>kindlykeyin@gmail.com</t>
+  </si>
+  <si>
+    <t>Keyin</t>
+  </si>
+  <si>
+    <t>CyDi</t>
+  </si>
+  <si>
+    <t>cydipl@gmail.com</t>
+  </si>
+  <si>
+    <t>Perichip</t>
+  </si>
+  <si>
+    <t>Aeroshiva</t>
+  </si>
+  <si>
+    <t>aeroshivagames@gmail.com</t>
+  </si>
+  <si>
+    <t>perichip@gmail.com</t>
+  </si>
+  <si>
+    <t>Cosmic Nava</t>
+  </si>
+  <si>
+    <t>beetje onduidelijk kanaal</t>
+  </si>
+  <si>
+    <t>Febatista</t>
+  </si>
+  <si>
+    <t>contatofebatista@gmail.com</t>
+  </si>
+  <si>
+    <t>Scyushi</t>
+  </si>
+  <si>
+    <t>Scy</t>
+  </si>
+  <si>
+    <t>scytheplays@gmail.com</t>
+  </si>
+  <si>
+    <t>Jerryn</t>
+  </si>
+  <si>
+    <t>jaroslav6@seznam.cz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tony.design04@gmail.com </t>
+  </si>
+  <si>
+    <t>Yomolotakowapo</t>
+  </si>
+  <si>
+    <t>business@yomolotakowapo.com</t>
+  </si>
+  <si>
+    <t>Caith_Sith</t>
+  </si>
+  <si>
+    <t>CaithYT@gmail.com</t>
+  </si>
+  <si>
+    <t>iTownGamePlay *Terror&amp;Diversión*</t>
+  </si>
+  <si>
+    <t>gameplaytown@hotmail.es</t>
+  </si>
+  <si>
+    <t>sSKENGSs</t>
+  </si>
+  <si>
+    <t>CYKER GAMER</t>
+  </si>
+  <si>
+    <t>КотоГеймер</t>
+  </si>
+  <si>
+    <t>MaKKowey Tapkin</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2088,6 +2334,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF606060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2116,7 +2368,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2151,6 +2403,8 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3416,13 +3670,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A25A688-B96F-4964-900E-15F95AB35B75}">
-  <dimension ref="A1:S313"/>
+  <dimension ref="A1:S355"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B231" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G336" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B244" sqref="B244"/>
+      <selection pane="bottomRight" activeCell="Q353" sqref="Q353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3561,6 +3815,9 @@
       <c r="K4">
         <v>1300</v>
       </c>
+      <c r="M4">
+        <v>2000</v>
+      </c>
       <c r="O4" s="13">
         <f t="shared" si="0"/>
         <v>1700</v>
@@ -3573,7 +3830,7 @@
       </c>
       <c r="S4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -4126,6 +4383,9 @@
       <c r="G29">
         <v>222</v>
       </c>
+      <c r="M29">
+        <v>56</v>
+      </c>
       <c r="O29" s="13">
         <f t="shared" si="0"/>
         <v>222</v>
@@ -4135,7 +4395,7 @@
       </c>
       <c r="S29">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
@@ -4738,6 +4998,9 @@
       <c r="K56">
         <v>1700</v>
       </c>
+      <c r="M56">
+        <v>477</v>
+      </c>
       <c r="O56" s="13">
         <f t="shared" si="0"/>
         <v>84</v>
@@ -4750,7 +5013,7 @@
       </c>
       <c r="S56">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.3">
@@ -4876,6 +5139,9 @@
       <c r="H62">
         <v>66</v>
       </c>
+      <c r="M62">
+        <v>5.2</v>
+      </c>
       <c r="O62" s="13">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -4885,7 +5151,7 @@
       </c>
       <c r="S62">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.3">
@@ -4907,6 +5173,9 @@
       <c r="J63">
         <v>25</v>
       </c>
+      <c r="M63">
+        <v>84</v>
+      </c>
       <c r="O63" s="13">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -4916,7 +5185,7 @@
       </c>
       <c r="S63">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.3">
@@ -5243,6 +5512,9 @@
       <c r="G78">
         <v>42</v>
       </c>
+      <c r="M78">
+        <v>43</v>
+      </c>
       <c r="O78" s="13">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -5252,7 +5524,7 @@
       </c>
       <c r="S78">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.3">
@@ -6233,6 +6505,9 @@
       <c r="B123">
         <v>9</v>
       </c>
+      <c r="M123">
+        <v>6.6</v>
+      </c>
       <c r="O123" s="13">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -6242,7 +6517,7 @@
       </c>
       <c r="S123">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.3">
@@ -6523,6 +6798,9 @@
       <c r="E137">
         <v>0.7</v>
       </c>
+      <c r="M137">
+        <v>2.1</v>
+      </c>
       <c r="O137" s="13">
         <f t="shared" si="4"/>
         <v>5.5</v>
@@ -6532,7 +6810,7 @@
       </c>
       <c r="S137">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.3">
@@ -6821,6 +7099,9 @@
       <c r="K153">
         <v>3.3</v>
       </c>
+      <c r="M153">
+        <v>2.1</v>
+      </c>
       <c r="O153" s="13">
         <f t="shared" si="4"/>
         <v>3.9</v>
@@ -6830,7 +7111,7 @@
       </c>
       <c r="S153">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="154" spans="1:19" x14ac:dyDescent="0.3">
@@ -7588,13 +7869,19 @@
       <c r="G197">
         <v>1.3</v>
       </c>
+      <c r="M197">
+        <v>2</v>
+      </c>
       <c r="O197" s="13">
         <f t="shared" si="6"/>
         <v>1.3</v>
       </c>
+      <c r="P197" s="9" t="s">
+        <v>719</v>
+      </c>
       <c r="S197">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="198" spans="1:19" x14ac:dyDescent="0.3">
@@ -8585,7 +8872,7 @@
         <v>0.3</v>
       </c>
       <c r="O257" s="13">
-        <f t="shared" ref="O257:O307" si="8">MAX(B257:J257)</f>
+        <f t="shared" ref="O257:O320" si="8">MAX(B257:J257)</f>
         <v>0.3</v>
       </c>
       <c r="S257">
@@ -8621,7 +8908,7 @@
         <v>0.3</v>
       </c>
       <c r="S259">
-        <f t="shared" ref="S259:S307" si="9">COUNTA(B259:N259)</f>
+        <f t="shared" ref="S259:S322" si="9">COUNTA(B259:N259)</f>
         <v>1</v>
       </c>
     </row>
@@ -9400,8 +9687,16 @@
       <c r="M308">
         <v>2200</v>
       </c>
+      <c r="O308" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="P308" s="9" t="s">
         <v>632</v>
+      </c>
+      <c r="S308">
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
     </row>
     <row r="309" spans="1:19" x14ac:dyDescent="0.3">
@@ -9411,8 +9706,16 @@
       <c r="M309">
         <v>5.4</v>
       </c>
+      <c r="O309" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="P309" s="9" t="s">
         <v>635</v>
+      </c>
+      <c r="S309">
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
     </row>
     <row r="310" spans="1:19" x14ac:dyDescent="0.3">
@@ -9425,8 +9728,16 @@
       <c r="M310">
         <v>24</v>
       </c>
+      <c r="O310" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="P310" s="8" t="s">
         <v>637</v>
+      </c>
+      <c r="S310">
+        <f t="shared" si="9"/>
+        <v>2</v>
       </c>
     </row>
     <row r="311" spans="1:19" x14ac:dyDescent="0.3">
@@ -9436,11 +9747,19 @@
       <c r="M311">
         <v>14</v>
       </c>
+      <c r="O311" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="P311" s="15" t="s">
         <v>640</v>
       </c>
       <c r="Q311" t="s">
         <v>638</v>
+      </c>
+      <c r="S311">
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
     </row>
     <row r="312" spans="1:19" x14ac:dyDescent="0.3">
@@ -9450,11 +9769,19 @@
       <c r="M312">
         <v>15</v>
       </c>
+      <c r="O312" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="P312" t="s">
         <v>642</v>
       </c>
       <c r="Q312" t="s">
         <v>643</v>
+      </c>
+      <c r="S312">
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
     </row>
     <row r="313" spans="1:19" x14ac:dyDescent="0.3">
@@ -9467,12 +9794,768 @@
       <c r="M313">
         <v>64</v>
       </c>
+      <c r="O313" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="P313" s="8" t="s">
         <v>646</v>
       </c>
       <c r="Q313" t="s">
         <v>645</v>
       </c>
+      <c r="S313">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="314" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A314" t="s">
+        <v>649</v>
+      </c>
+      <c r="M314">
+        <v>2.1</v>
+      </c>
+      <c r="O314" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P314" t="s">
+        <v>499</v>
+      </c>
+      <c r="R314" t="s">
+        <v>613</v>
+      </c>
+      <c r="S314">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A315" t="s">
+        <v>650</v>
+      </c>
+      <c r="M315">
+        <v>79</v>
+      </c>
+      <c r="O315" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P315" s="8" t="s">
+        <v>651</v>
+      </c>
+      <c r="S315">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A316" t="s">
+        <v>652</v>
+      </c>
+      <c r="K316">
+        <v>85</v>
+      </c>
+      <c r="L316">
+        <v>52</v>
+      </c>
+      <c r="M316">
+        <v>60</v>
+      </c>
+      <c r="O316" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P316" t="s">
+        <v>653</v>
+      </c>
+      <c r="S316">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="317" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A317" t="s">
+        <v>654</v>
+      </c>
+      <c r="G317">
+        <v>7.4</v>
+      </c>
+      <c r="M317">
+        <v>14</v>
+      </c>
+      <c r="O317" s="13">
+        <f t="shared" si="8"/>
+        <v>7.4</v>
+      </c>
+      <c r="P317" t="s">
+        <v>655</v>
+      </c>
+      <c r="S317">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="318" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A318" t="s">
+        <v>656</v>
+      </c>
+      <c r="K318">
+        <v>1900</v>
+      </c>
+      <c r="M318">
+        <v>235</v>
+      </c>
+      <c r="O318" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P318" t="s">
+        <v>657</v>
+      </c>
+      <c r="S318">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="319" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A319" t="s">
+        <v>658</v>
+      </c>
+      <c r="F319">
+        <v>50</v>
+      </c>
+      <c r="L319">
+        <v>37</v>
+      </c>
+      <c r="M319">
+        <v>1.3</v>
+      </c>
+      <c r="O319" s="13">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="P319" s="8" t="s">
+        <v>659</v>
+      </c>
+      <c r="S319">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="320" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A320" t="s">
+        <v>660</v>
+      </c>
+      <c r="M320">
+        <v>148</v>
+      </c>
+      <c r="O320" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P320" s="8" t="s">
+        <v>661</v>
+      </c>
+      <c r="S320">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A321" t="s">
+        <v>662</v>
+      </c>
+      <c r="M321">
+        <v>3</v>
+      </c>
+      <c r="O321" s="13">
+        <f t="shared" ref="O321:O326" si="10">MAX(B321:J321)</f>
+        <v>0</v>
+      </c>
+      <c r="P321" s="8" t="s">
+        <v>663</v>
+      </c>
+      <c r="S321">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A322" t="s">
+        <v>664</v>
+      </c>
+      <c r="M322">
+        <v>45</v>
+      </c>
+      <c r="O322" s="13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P322" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="S322">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A323" t="s">
+        <v>666</v>
+      </c>
+      <c r="M323">
+        <v>5.3</v>
+      </c>
+      <c r="O323" s="13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P323" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="R323" t="s">
+        <v>613</v>
+      </c>
+      <c r="S323">
+        <f t="shared" ref="S323:S354" si="11">COUNTA(B323:N323)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A324" t="s">
+        <v>667</v>
+      </c>
+      <c r="M324">
+        <v>7.6</v>
+      </c>
+      <c r="O324" s="13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P324" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="S324">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A325" t="s">
+        <v>669</v>
+      </c>
+      <c r="K325">
+        <v>305</v>
+      </c>
+      <c r="M325">
+        <v>1.5</v>
+      </c>
+      <c r="O325" s="13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P325" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="S325">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="326" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A326" t="s">
+        <v>671</v>
+      </c>
+      <c r="M326">
+        <v>1.9</v>
+      </c>
+      <c r="O326" s="13">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P326" t="s">
+        <v>673</v>
+      </c>
+      <c r="Q326" t="s">
+        <v>672</v>
+      </c>
+      <c r="S326">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="327" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A327" t="s">
+        <v>674</v>
+      </c>
+      <c r="M327">
+        <v>1.9</v>
+      </c>
+      <c r="P327" t="s">
+        <v>675</v>
+      </c>
+      <c r="S327">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="328" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A328" t="s">
+        <v>676</v>
+      </c>
+      <c r="M328">
+        <v>3.3</v>
+      </c>
+      <c r="P328" t="s">
+        <v>677</v>
+      </c>
+      <c r="S328">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A329" t="s">
+        <v>678</v>
+      </c>
+      <c r="M329">
+        <v>2.7</v>
+      </c>
+      <c r="P329" t="s">
+        <v>679</v>
+      </c>
+      <c r="Q329" t="s">
+        <v>680</v>
+      </c>
+      <c r="S329">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A330" t="s">
+        <v>681</v>
+      </c>
+      <c r="M330">
+        <v>2</v>
+      </c>
+      <c r="P330" t="s">
+        <v>682</v>
+      </c>
+      <c r="S330">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A331" t="s">
+        <v>683</v>
+      </c>
+      <c r="K331">
+        <v>1.3</v>
+      </c>
+      <c r="M331">
+        <v>2</v>
+      </c>
+      <c r="P331" s="8" t="s">
+        <v>684</v>
+      </c>
+      <c r="S331">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="332" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A332" t="s">
+        <v>685</v>
+      </c>
+      <c r="M332">
+        <v>3</v>
+      </c>
+      <c r="P332" t="s">
+        <v>686</v>
+      </c>
+      <c r="S332">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="333" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A333" t="s">
+        <v>687</v>
+      </c>
+      <c r="K333">
+        <v>519</v>
+      </c>
+      <c r="M333">
+        <v>130</v>
+      </c>
+      <c r="P333" s="8" t="s">
+        <v>688</v>
+      </c>
+      <c r="S333">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="334" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A334" t="s">
+        <v>689</v>
+      </c>
+      <c r="M334">
+        <v>3.7</v>
+      </c>
+      <c r="P334" s="9" t="s">
+        <v>690</v>
+      </c>
+      <c r="S334">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A335" t="s">
+        <v>691</v>
+      </c>
+      <c r="M335">
+        <v>1.9</v>
+      </c>
+      <c r="P335" t="s">
+        <v>531</v>
+      </c>
+      <c r="S335">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="336" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A336" t="s">
+        <v>694</v>
+      </c>
+      <c r="M336">
+        <v>2.8</v>
+      </c>
+      <c r="P336" s="8" t="s">
+        <v>692</v>
+      </c>
+      <c r="Q336" t="s">
+        <v>693</v>
+      </c>
+      <c r="S336">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A337" t="s">
+        <v>695</v>
+      </c>
+      <c r="M337">
+        <v>1.2</v>
+      </c>
+      <c r="P337" t="s">
+        <v>499</v>
+      </c>
+      <c r="R337" t="s">
+        <v>696</v>
+      </c>
+      <c r="S337">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="338" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A338" t="s">
+        <v>697</v>
+      </c>
+      <c r="F338">
+        <v>314</v>
+      </c>
+      <c r="M338">
+        <v>93</v>
+      </c>
+      <c r="P338" s="8" t="s">
+        <v>698</v>
+      </c>
+      <c r="S338">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="339" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A339" t="s">
+        <v>700</v>
+      </c>
+      <c r="M339">
+        <v>3.1</v>
+      </c>
+      <c r="P339" t="s">
+        <v>699</v>
+      </c>
+      <c r="S339">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="340" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A340" t="s">
+        <v>701</v>
+      </c>
+      <c r="F340">
+        <v>116</v>
+      </c>
+      <c r="M340">
+        <v>15</v>
+      </c>
+      <c r="P340" s="8" t="s">
+        <v>702</v>
+      </c>
+      <c r="Q340" t="s">
+        <v>703</v>
+      </c>
+      <c r="S340">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="341" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A341" t="s">
+        <v>704</v>
+      </c>
+      <c r="M341">
+        <v>13</v>
+      </c>
+      <c r="P341" t="s">
+        <v>705</v>
+      </c>
+      <c r="S341">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="342" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A342" t="s">
+        <v>706</v>
+      </c>
+      <c r="M342">
+        <v>23</v>
+      </c>
+      <c r="P342" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="S342">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="343" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A343" t="s">
+        <v>707</v>
+      </c>
+      <c r="M343">
+        <v>5.3</v>
+      </c>
+      <c r="P343" t="s">
+        <v>708</v>
+      </c>
+      <c r="S343">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A344" t="s">
+        <v>710</v>
+      </c>
+      <c r="M344">
+        <v>6.7</v>
+      </c>
+      <c r="R344" t="s">
+        <v>711</v>
+      </c>
+      <c r="S344">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A345" t="s">
+        <v>712</v>
+      </c>
+      <c r="K345">
+        <v>302</v>
+      </c>
+      <c r="M345">
+        <v>139</v>
+      </c>
+      <c r="P345" s="9" t="s">
+        <v>713</v>
+      </c>
+      <c r="S345">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="346" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A346" t="s">
+        <v>714</v>
+      </c>
+      <c r="M346">
+        <v>4</v>
+      </c>
+      <c r="P346" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q346" t="s">
+        <v>715</v>
+      </c>
+      <c r="S346">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A347" t="s">
+        <v>717</v>
+      </c>
+      <c r="F347">
+        <v>2.6</v>
+      </c>
+      <c r="K347">
+        <v>44</v>
+      </c>
+      <c r="M347">
+        <v>6.3</v>
+      </c>
+      <c r="P347" t="s">
+        <v>718</v>
+      </c>
+      <c r="S347">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="348" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
+        <v>720</v>
+      </c>
+      <c r="M348">
+        <v>3.2</v>
+      </c>
+      <c r="P348" s="8" t="s">
+        <v>721</v>
+      </c>
+      <c r="S348">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="349" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
+        <v>722</v>
+      </c>
+      <c r="M349">
+        <v>5</v>
+      </c>
+      <c r="P349" s="8" t="s">
+        <v>723</v>
+      </c>
+      <c r="S349">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="350" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A350" t="s">
+        <v>724</v>
+      </c>
+      <c r="K350">
+        <v>574</v>
+      </c>
+      <c r="M350">
+        <v>666</v>
+      </c>
+      <c r="P350" t="s">
+        <v>725</v>
+      </c>
+      <c r="S350">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="351" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A351" t="s">
+        <v>726</v>
+      </c>
+      <c r="M351">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="P351" t="s">
+        <v>730</v>
+      </c>
+      <c r="S351">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="352" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A352" t="s">
+        <v>727</v>
+      </c>
+      <c r="M352">
+        <v>26</v>
+      </c>
+      <c r="P352" t="s">
+        <v>499</v>
+      </c>
+      <c r="R352" t="s">
+        <v>613</v>
+      </c>
+      <c r="S352">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
+        <v>728</v>
+      </c>
+      <c r="K353">
+        <v>0.1</v>
+      </c>
+      <c r="M353">
+        <v>7.3</v>
+      </c>
+      <c r="P353" t="s">
+        <v>730</v>
+      </c>
+      <c r="S353">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="354" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
+        <v>729</v>
+      </c>
+      <c r="K354">
+        <v>7.3</v>
+      </c>
+      <c r="M354">
+        <v>10</v>
+      </c>
+      <c r="P354" t="s">
+        <v>730</v>
+      </c>
+      <c r="S354">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="355" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A355" s="17"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:R1" xr:uid="{9448E0E4-6782-4C8B-9CFC-41FF34BC7D4A}">
@@ -9505,9 +10588,11 @@
     <hyperlink ref="P51" r:id="rId19" xr:uid="{2B53BAFF-12E2-4F40-B2D1-70A2B1F51CFC}"/>
     <hyperlink ref="P55" r:id="rId20" display="mailto:gilathiss.biznes@gmail.com" xr:uid="{ADFA18F4-F2AA-4DDF-A139-7D0E93BD3284}"/>
     <hyperlink ref="P133" r:id="rId21" xr:uid="{5683E5CE-306D-43C0-8A77-611187A6EEE3}"/>
+    <hyperlink ref="P322" r:id="rId22" display="mailto:jpad17officialchannel@gmail.com" xr:uid="{B7CEEDA3-E05A-4CBE-8C23-A14DADDBBCBD}"/>
+    <hyperlink ref="P342" r:id="rId23" xr:uid="{D3533793-9177-4AE8-AC1A-C82254C65329}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Workign on marketing plan
</commit_message>
<xml_diff>
--- a/Marketing planning.xlsx
+++ b/Marketing planning.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wessel\Desktop\thesapling-website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wstoop\Documents\thesapling-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B10E156-864A-4873-878C-E0724E2B7E79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="782" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overzicht" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Filmpjesmakers!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Nieuwe Youtubers'!$A$1:$R$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="756">
   <si>
     <t>Week</t>
   </si>
@@ -2303,11 +2304,44 @@
   <si>
     <t>unity3d</t>
   </si>
+  <si>
+    <t>Times</t>
+  </si>
+  <si>
+    <t>2:30 'which is quite exciting', 2:48 'someone carrying shopping bags', 7:38 'yes it's perfect', 32:18 *laugh* 'this is the best creature', 43:53 'look it has little tiny feet this is brilliant', 51:53 'it is a lot of fun to play'</t>
+  </si>
+  <si>
+    <t>7:38 'oh yeah yeah yeah', 12:28 'there's a lot of animals out here, you know what that means… it's carnivore time'</t>
+  </si>
+  <si>
+    <t>no commentary, not watched</t>
+  </si>
+  <si>
+    <t>speedrun</t>
+  </si>
+  <si>
+    <t>0:08 'very sandboxy, very cool', 3:38 'really really cool', 18:31 'I really enjoy this, designing my own plants, making them look cool', 24:10 'how super interesting is this', 44:02 'this has been really really cool just to play around with', 44:14 'it's super fun just playing around with all the little bits and pieces and different leaves and see what you can do with it'</t>
+  </si>
+  <si>
+    <t>maakt ook 'upcoming' filmpjes</t>
+  </si>
+  <si>
+    <t>7:05 'there we go, ooooh' 9:40 'ooooh wow there' 9:48 'okay i was no expecting that, that did make me jump', 15:45 'yes yes... oh this is gonna be a monstrous looking plant'</t>
+  </si>
+  <si>
+    <t>1:08 'ooh that looks good', 10:10 'ooh we get a baby up here… ooh pause pause pause', 18:35 'ooh look at that xaro has a new tail', 18:55 'that looks actually quite cool', 19:36 'it's a lotta fun'</t>
+  </si>
+  <si>
+    <t>0:26 'yes oohoohooo we got lots of roots there', 1:56 'wow wow wow we got a lotta green baby plants, that's awesome… look at them go!', 3:30 'woow this is really cool', 5:44 'ooh they turned into woody plants… wow!'</t>
+  </si>
+  <si>
+    <t>1:48 'I love the music, absolutely love the music', 2:22 'I love these graphics… they're simple, they're cute and they're wonderful… so I'm very excited, the music very fitting'</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2449,7 +2483,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2760,7 +2794,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2770,20 +2804,20 @@
       <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="20.5703125" style="1"/>
-    <col min="8" max="8" width="20.5703125" style="1"/>
-    <col min="11" max="16" width="20.5703125" style="1"/>
-    <col min="17" max="17" width="11.28515625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5703125" style="1"/>
-    <col min="21" max="16384" width="20.5703125" style="1"/>
+    <col min="1" max="1" width="14.33203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="20.5546875" style="1"/>
+    <col min="8" max="8" width="20.5546875" style="1"/>
+    <col min="11" max="16" width="20.5546875" style="1"/>
+    <col min="17" max="17" width="11.33203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="20.5546875" style="1"/>
+    <col min="21" max="16384" width="20.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="6" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
@@ -2848,7 +2882,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>40</v>
       </c>
@@ -2865,7 +2899,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
@@ -2884,7 +2918,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>42</v>
       </c>
@@ -2903,7 +2937,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>43</v>
       </c>
@@ -2925,7 +2959,7 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>44</v>
       </c>
@@ -2944,7 +2978,7 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>45</v>
       </c>
@@ -2963,7 +2997,7 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>46</v>
       </c>
@@ -2985,7 +3019,7 @@
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>47</v>
       </c>
@@ -3041,7 +3075,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>48</v>
       </c>
@@ -3066,7 +3100,7 @@
       <c r="J10" s="1"/>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
@@ -3091,7 +3125,7 @@
       <c r="J11" s="1"/>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
@@ -3116,7 +3150,7 @@
       <c r="J12" s="1"/>
       <c r="K12"/>
     </row>
-    <row r="13" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>51</v>
       </c>
@@ -3144,7 +3178,7 @@
       <c r="J13" s="1"/>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>52</v>
       </c>
@@ -3200,7 +3234,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
@@ -3227,36 +3261,36 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>744</v>
       </c>
@@ -3267,24 +3301,24 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -3295,16 +3329,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -3315,14 +3349,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -3333,32 +3367,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -3371,8 +3405,11 @@
       <c r="D1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -3382,8 +3419,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -3393,8 +3433,11 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -3404,8 +3447,11 @@
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -3416,7 +3462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -3426,8 +3472,11 @@
       <c r="C6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -3437,8 +3486,11 @@
       <c r="C7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -3448,8 +3500,11 @@
       <c r="C8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>102</v>
       </c>
@@ -3463,7 +3518,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>91</v>
       </c>
@@ -3473,8 +3528,11 @@
       <c r="C10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>99</v>
       </c>
@@ -3488,7 +3546,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -3498,8 +3556,11 @@
       <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>95</v>
       </c>
@@ -3509,8 +3570,11 @@
       <c r="C13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>98</v>
       </c>
@@ -3520,8 +3584,11 @@
       <c r="C14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>97</v>
       </c>
@@ -3531,8 +3598,11 @@
       <c r="C15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>96</v>
       </c>
@@ -3542,8 +3612,11 @@
       <c r="C16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -3553,10 +3626,13 @@
       <c r="C17">
         <v>1</v>
       </c>
+      <c r="D17" t="s">
+        <v>748</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1">
-    <sortState ref="A2:D17">
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000004000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D17">
       <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>
@@ -3565,141 +3641,141 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:A34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>349</v>
       </c>
@@ -3710,34 +3786,34 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S355"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G183" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G90" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R214" sqref="R214"/>
+      <selection pane="bottomRight" activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="21" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.28515625" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>163</v>
       </c>
@@ -3796,7 +3872,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>174</v>
       </c>
@@ -3821,7 +3897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>105</v>
       </c>
@@ -3846,7 +3922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>236</v>
       </c>
@@ -3874,7 +3950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -3902,7 +3978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>357</v>
       </c>
@@ -3924,7 +4000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>415</v>
       </c>
@@ -3946,7 +4022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>232</v>
       </c>
@@ -3968,7 +4044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>207</v>
       </c>
@@ -3990,7 +4066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>181</v>
       </c>
@@ -4012,7 +4088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>366</v>
       </c>
@@ -4034,7 +4110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>372</v>
       </c>
@@ -4056,7 +4132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>371</v>
       </c>
@@ -4078,7 +4154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>359</v>
       </c>
@@ -4097,7 +4173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>350</v>
       </c>
@@ -4119,7 +4195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>291</v>
       </c>
@@ -4144,7 +4220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>354</v>
       </c>
@@ -4172,7 +4248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>120</v>
       </c>
@@ -4194,7 +4270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>360</v>
       </c>
@@ -4216,7 +4292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>375</v>
       </c>
@@ -4235,7 +4311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>313</v>
       </c>
@@ -4254,7 +4330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>256</v>
       </c>
@@ -4279,7 +4355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>399</v>
       </c>
@@ -4295,7 +4371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>318</v>
       </c>
@@ -4320,7 +4396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -4342,7 +4418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>248</v>
       </c>
@@ -4370,7 +4446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>177</v>
       </c>
@@ -4395,7 +4471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>355</v>
       </c>
@@ -4417,7 +4493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>187</v>
       </c>
@@ -4439,7 +4515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>192</v>
       </c>
@@ -4458,7 +4534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>226</v>
       </c>
@@ -4480,7 +4556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>136</v>
       </c>
@@ -4499,7 +4575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>178</v>
       </c>
@@ -4521,7 +4597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>287</v>
       </c>
@@ -4546,7 +4622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>353</v>
       </c>
@@ -4571,7 +4647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>257</v>
       </c>
@@ -4599,7 +4675,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>292</v>
       </c>
@@ -4624,7 +4700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>195</v>
       </c>
@@ -4646,7 +4722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>289</v>
       </c>
@@ -4668,7 +4744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>244</v>
       </c>
@@ -4696,7 +4772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>188</v>
       </c>
@@ -4721,7 +4797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>175</v>
       </c>
@@ -4746,7 +4822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>206</v>
       </c>
@@ -4768,7 +4844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>525</v>
       </c>
@@ -4790,7 +4866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>115</v>
       </c>
@@ -4815,7 +4891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>258</v>
       </c>
@@ -4834,7 +4910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>264</v>
       </c>
@@ -4853,7 +4929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>274</v>
       </c>
@@ -4881,7 +4957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>176</v>
       </c>
@@ -4903,7 +4979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>240</v>
       </c>
@@ -4928,7 +5004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>401</v>
       </c>
@@ -4947,7 +5023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>259</v>
       </c>
@@ -4969,7 +5045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -4988,7 +5064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>423</v>
       </c>
@@ -5010,7 +5086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>351</v>
       </c>
@@ -5029,7 +5105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>364</v>
       </c>
@@ -5057,7 +5133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>194</v>
       </c>
@@ -5076,7 +5152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>231</v>
       </c>
@@ -5101,7 +5177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>180</v>
       </c>
@@ -5123,7 +5199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>367</v>
       </c>
@@ -5148,7 +5224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>365</v>
       </c>
@@ -5170,7 +5246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>209</v>
       </c>
@@ -5195,7 +5271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>117</v>
       </c>
@@ -5229,7 +5305,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>395</v>
       </c>
@@ -5254,7 +5330,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>266</v>
       </c>
@@ -5279,7 +5355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>238</v>
       </c>
@@ -5298,7 +5374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>242</v>
       </c>
@@ -5317,7 +5393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>434</v>
       </c>
@@ -5339,7 +5415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>218</v>
       </c>
@@ -5358,7 +5434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>299</v>
       </c>
@@ -5386,7 +5462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>388</v>
       </c>
@@ -5414,7 +5490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>315</v>
       </c>
@@ -5436,7 +5512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>276</v>
       </c>
@@ -5458,7 +5534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>196</v>
       </c>
@@ -5480,7 +5556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>283</v>
       </c>
@@ -5499,7 +5575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>179</v>
       </c>
@@ -5527,7 +5603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>169</v>
       </c>
@@ -5546,7 +5622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>183</v>
       </c>
@@ -5568,7 +5644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>290</v>
       </c>
@@ -5596,7 +5672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>182</v>
       </c>
@@ -5621,7 +5697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>282</v>
       </c>
@@ -5640,7 +5716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>141</v>
       </c>
@@ -5659,7 +5735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>211</v>
       </c>
@@ -5681,7 +5757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>106</v>
       </c>
@@ -5703,7 +5779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>133</v>
       </c>
@@ -5725,7 +5801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>223</v>
       </c>
@@ -5744,7 +5820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>272</v>
       </c>
@@ -5763,7 +5839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>386</v>
       </c>
@@ -5782,7 +5858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>199</v>
       </c>
@@ -5807,7 +5883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>198</v>
       </c>
@@ -5829,7 +5905,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>201</v>
       </c>
@@ -5854,7 +5930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>277</v>
       </c>
@@ -5879,7 +5955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>171</v>
       </c>
@@ -5898,7 +5974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>190</v>
       </c>
@@ -5917,7 +5993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>189</v>
       </c>
@@ -5939,7 +6015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>368</v>
       </c>
@@ -5958,7 +6034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>419</v>
       </c>
@@ -5983,7 +6059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>230</v>
       </c>
@@ -6002,7 +6078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>361</v>
       </c>
@@ -6024,7 +6100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>197</v>
       </c>
@@ -6049,7 +6125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>408</v>
       </c>
@@ -6071,7 +6147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>220</v>
       </c>
@@ -6090,7 +6166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>227</v>
       </c>
@@ -6110,12 +6186,15 @@
       <c r="Q103" t="s">
         <v>568</v>
       </c>
+      <c r="R103" t="s">
+        <v>751</v>
+      </c>
       <c r="S103">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>253</v>
       </c>
@@ -6134,7 +6213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>404</v>
       </c>
@@ -6156,7 +6235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>212</v>
       </c>
@@ -6175,7 +6254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>260</v>
       </c>
@@ -6197,7 +6276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>358</v>
       </c>
@@ -6222,7 +6301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>229</v>
       </c>
@@ -6244,7 +6323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>204</v>
       </c>
@@ -6269,7 +6348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>132</v>
       </c>
@@ -6294,7 +6373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>210</v>
       </c>
@@ -6319,7 +6398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>233</v>
       </c>
@@ -6341,7 +6420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>284</v>
       </c>
@@ -6366,7 +6445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>426</v>
       </c>
@@ -6388,7 +6467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>221</v>
       </c>
@@ -6410,7 +6489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>247</v>
       </c>
@@ -6435,7 +6514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>252</v>
       </c>
@@ -6457,7 +6536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>108</v>
       </c>
@@ -6479,7 +6558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>186</v>
       </c>
@@ -6501,7 +6580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>235</v>
       </c>
@@ -6523,7 +6602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>200</v>
       </c>
@@ -6542,7 +6621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>111</v>
       </c>
@@ -6564,7 +6643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>304</v>
       </c>
@@ -6583,7 +6662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>234</v>
       </c>
@@ -6608,7 +6687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>128</v>
       </c>
@@ -6630,7 +6709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>295</v>
       </c>
@@ -6649,7 +6728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>403</v>
       </c>
@@ -6668,7 +6747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>263</v>
       </c>
@@ -6690,7 +6769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>429</v>
       </c>
@@ -6709,7 +6788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>245</v>
       </c>
@@ -6731,7 +6810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>320</v>
       </c>
@@ -6753,7 +6832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>407</v>
       </c>
@@ -6772,7 +6851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>184</v>
       </c>
@@ -6791,7 +6870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>213</v>
       </c>
@@ -6810,7 +6889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>356</v>
       </c>
@@ -6832,7 +6911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>126</v>
       </c>
@@ -6857,7 +6936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>219</v>
       </c>
@@ -6879,7 +6958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>123</v>
       </c>
@@ -6901,7 +6980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>203</v>
       </c>
@@ -6920,7 +6999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>112</v>
       </c>
@@ -6939,7 +7018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>130</v>
       </c>
@@ -6958,7 +7037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>140</v>
       </c>
@@ -6977,7 +7056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>216</v>
       </c>
@@ -6993,7 +7072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>228</v>
       </c>
@@ -7009,7 +7088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>271</v>
       </c>
@@ -7025,7 +7104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>110</v>
       </c>
@@ -7044,7 +7123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>352</v>
       </c>
@@ -7060,7 +7139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>414</v>
       </c>
@@ -7076,7 +7155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>113</v>
       </c>
@@ -7098,7 +7177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>267</v>
       </c>
@@ -7114,7 +7193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>316</v>
       </c>
@@ -7130,7 +7209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>150</v>
       </c>
@@ -7158,7 +7237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>383</v>
       </c>
@@ -7174,7 +7253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>322</v>
       </c>
@@ -7190,7 +7269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>165</v>
       </c>
@@ -7212,7 +7291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>118</v>
       </c>
@@ -7234,7 +7313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>268</v>
       </c>
@@ -7250,7 +7329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>405</v>
       </c>
@@ -7266,7 +7345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>255</v>
       </c>
@@ -7282,7 +7361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>278</v>
       </c>
@@ -7298,7 +7377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>273</v>
       </c>
@@ -7314,7 +7393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>373</v>
       </c>
@@ -7330,7 +7409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>191</v>
       </c>
@@ -7346,7 +7425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>249</v>
       </c>
@@ -7362,7 +7441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>396</v>
       </c>
@@ -7378,7 +7457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>124</v>
       </c>
@@ -7400,7 +7479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>170</v>
       </c>
@@ -7416,7 +7495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>243</v>
       </c>
@@ -7432,7 +7511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>307</v>
       </c>
@@ -7448,7 +7527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>125</v>
       </c>
@@ -7470,7 +7549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>122</v>
       </c>
@@ -7489,7 +7568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>185</v>
       </c>
@@ -7505,7 +7584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>202</v>
       </c>
@@ -7521,7 +7600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>285</v>
       </c>
@@ -7537,7 +7616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>286</v>
       </c>
@@ -7562,7 +7641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>139</v>
       </c>
@@ -7581,7 +7660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>193</v>
       </c>
@@ -7597,7 +7676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>296</v>
       </c>
@@ -7613,7 +7692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>297</v>
       </c>
@@ -7629,7 +7708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>412</v>
       </c>
@@ -7645,7 +7724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>215</v>
       </c>
@@ -7661,7 +7740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>225</v>
       </c>
@@ -7677,7 +7756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>389</v>
       </c>
@@ -7693,7 +7772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>431</v>
       </c>
@@ -7709,7 +7788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>138</v>
       </c>
@@ -7728,7 +7807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>317</v>
       </c>
@@ -7753,7 +7832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>387</v>
       </c>
@@ -7769,7 +7848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>137</v>
       </c>
@@ -7788,7 +7867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>222</v>
       </c>
@@ -7804,7 +7883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>241</v>
       </c>
@@ -7820,7 +7899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>319</v>
       </c>
@@ -7836,7 +7915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>321</v>
       </c>
@@ -7852,7 +7931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>323</v>
       </c>
@@ -7868,7 +7947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>324</v>
       </c>
@@ -7884,7 +7963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>116</v>
       </c>
@@ -7906,7 +7985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>224</v>
       </c>
@@ -7928,7 +8007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>302</v>
       </c>
@@ -7944,7 +8023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>119</v>
       </c>
@@ -7966,7 +8045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>148</v>
       </c>
@@ -7988,7 +8067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>164</v>
       </c>
@@ -8007,7 +8086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>424</v>
       </c>
@@ -8023,7 +8102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>433</v>
       </c>
@@ -8039,7 +8118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>246</v>
       </c>
@@ -8055,7 +8134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>275</v>
       </c>
@@ -8071,7 +8150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>281</v>
       </c>
@@ -8087,7 +8166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>310</v>
       </c>
@@ -8103,7 +8182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>390</v>
       </c>
@@ -8119,7 +8198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>393</v>
       </c>
@@ -8135,7 +8214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>166</v>
       </c>
@@ -8160,7 +8239,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="211" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>301</v>
       </c>
@@ -8176,7 +8255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>311</v>
       </c>
@@ -8192,7 +8271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>436</v>
       </c>
@@ -8208,7 +8287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>134</v>
       </c>
@@ -8233,7 +8312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>154</v>
       </c>
@@ -8249,7 +8328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>153</v>
       </c>
@@ -8265,7 +8344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>94</v>
       </c>
@@ -8281,7 +8360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>265</v>
       </c>
@@ -8297,7 +8376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>300</v>
       </c>
@@ -8313,7 +8392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>314</v>
       </c>
@@ -8329,7 +8408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>370</v>
       </c>
@@ -8345,7 +8424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>382</v>
       </c>
@@ -8361,7 +8440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>397</v>
       </c>
@@ -8377,7 +8456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>144</v>
       </c>
@@ -8393,7 +8472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>147</v>
       </c>
@@ -8409,7 +8488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>262</v>
       </c>
@@ -8425,7 +8504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>288</v>
       </c>
@@ -8441,7 +8520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>303</v>
       </c>
@@ -8457,7 +8536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>312</v>
       </c>
@@ -8473,7 +8552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>152</v>
       </c>
@@ -8489,7 +8568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>309</v>
       </c>
@@ -8505,7 +8584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>400</v>
       </c>
@@ -8521,7 +8600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>129</v>
       </c>
@@ -8537,7 +8616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>146</v>
       </c>
@@ -8553,7 +8632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>149</v>
       </c>
@@ -8569,7 +8648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>279</v>
       </c>
@@ -8585,7 +8664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>402</v>
       </c>
@@ -8601,7 +8680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>107</v>
       </c>
@@ -8617,7 +8696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>151</v>
       </c>
@@ -8633,7 +8712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>308</v>
       </c>
@@ -8649,7 +8728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>381</v>
       </c>
@@ -8665,7 +8744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>394</v>
       </c>
@@ -8681,7 +8760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>410</v>
       </c>
@@ -8697,7 +8776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>413</v>
       </c>
@@ -8722,7 +8801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>208</v>
       </c>
@@ -8738,7 +8817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>214</v>
       </c>
@@ -8754,7 +8833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>217</v>
       </c>
@@ -8770,7 +8849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>237</v>
       </c>
@@ -8786,7 +8865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>239</v>
       </c>
@@ -8802,7 +8881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>254</v>
       </c>
@@ -8818,7 +8897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>261</v>
       </c>
@@ -8834,7 +8913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>293</v>
       </c>
@@ -8850,7 +8929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>305</v>
       </c>
@@ -8866,7 +8945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>306</v>
       </c>
@@ -8882,7 +8961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>378</v>
       </c>
@@ -8898,7 +8977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>391</v>
       </c>
@@ -8914,7 +8993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>406</v>
       </c>
@@ -8930,7 +9009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>411</v>
       </c>
@@ -8946,7 +9025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>416</v>
       </c>
@@ -8962,7 +9041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>421</v>
       </c>
@@ -8978,7 +9057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>428</v>
       </c>
@@ -8994,7 +9073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>439</v>
       </c>
@@ -9010,7 +9089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>409</v>
       </c>
@@ -9026,7 +9105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>121</v>
       </c>
@@ -9042,7 +9121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>167</v>
       </c>
@@ -9058,7 +9137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>173</v>
       </c>
@@ -9074,7 +9153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>205</v>
       </c>
@@ -9090,7 +9169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>250</v>
       </c>
@@ -9106,7 +9185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>251</v>
       </c>
@@ -9122,7 +9201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>294</v>
       </c>
@@ -9138,7 +9217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>363</v>
       </c>
@@ -9154,7 +9233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>376</v>
       </c>
@@ -9170,7 +9249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>379</v>
       </c>
@@ -9186,7 +9265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>384</v>
       </c>
@@ -9202,7 +9281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>392</v>
       </c>
@@ -9218,7 +9297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>398</v>
       </c>
@@ -9234,7 +9313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>417</v>
       </c>
@@ -9250,7 +9329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>418</v>
       </c>
@@ -9266,7 +9345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>420</v>
       </c>
@@ -9282,7 +9361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>422</v>
       </c>
@@ -9298,7 +9377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>427</v>
       </c>
@@ -9314,7 +9393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>437</v>
       </c>
@@ -9330,7 +9409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>438</v>
       </c>
@@ -9346,7 +9425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>441</v>
       </c>
@@ -9362,7 +9441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>442</v>
       </c>
@@ -9378,7 +9457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>443</v>
       </c>
@@ -9394,7 +9473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>114</v>
       </c>
@@ -9410,7 +9489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>135</v>
       </c>
@@ -9426,7 +9505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>142</v>
       </c>
@@ -9442,7 +9521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>143</v>
       </c>
@@ -9458,7 +9537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>145</v>
       </c>
@@ -9474,7 +9553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>269</v>
       </c>
@@ -9490,7 +9569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>270</v>
       </c>
@@ -9506,7 +9585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>280</v>
       </c>
@@ -9522,7 +9601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>298</v>
       </c>
@@ -9538,7 +9617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>362</v>
       </c>
@@ -9554,7 +9633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>369</v>
       </c>
@@ -9570,7 +9649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>374</v>
       </c>
@@ -9586,7 +9665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>377</v>
       </c>
@@ -9602,7 +9681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>380</v>
       </c>
@@ -9618,7 +9697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>385</v>
       </c>
@@ -9634,7 +9713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>425</v>
       </c>
@@ -9650,7 +9729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>430</v>
       </c>
@@ -9666,7 +9745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>432</v>
       </c>
@@ -9682,7 +9761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>435</v>
       </c>
@@ -9698,7 +9777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>440</v>
       </c>
@@ -9714,7 +9793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>168</v>
       </c>
@@ -9730,7 +9809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>631</v>
       </c>
@@ -9749,7 +9828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>632</v>
       </c>
@@ -9768,7 +9847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>634</v>
       </c>
@@ -9790,7 +9869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="311" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>637</v>
       </c>
@@ -9812,7 +9891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>639</v>
       </c>
@@ -9834,7 +9913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>642</v>
       </c>
@@ -9859,7 +9938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="314" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>647</v>
       </c>
@@ -9881,7 +9960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>648</v>
       </c>
@@ -9900,7 +9979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>650</v>
       </c>
@@ -9925,7 +10004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="317" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>652</v>
       </c>
@@ -9947,7 +10026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>654</v>
       </c>
@@ -9969,7 +10048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="319" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>656</v>
       </c>
@@ -9994,7 +10073,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="320" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>658</v>
       </c>
@@ -10013,7 +10092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>660</v>
       </c>
@@ -10032,7 +10111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>662</v>
       </c>
@@ -10051,7 +10130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>664</v>
       </c>
@@ -10073,7 +10152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>665</v>
       </c>
@@ -10092,7 +10171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>667</v>
       </c>
@@ -10114,7 +10193,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="326" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>669</v>
       </c>
@@ -10136,7 +10215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>672</v>
       </c>
@@ -10151,7 +10230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>674</v>
       </c>
@@ -10166,7 +10245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>676</v>
       </c>
@@ -10184,7 +10263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>679</v>
       </c>
@@ -10199,7 +10278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>681</v>
       </c>
@@ -10217,7 +10296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="332" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>683</v>
       </c>
@@ -10232,7 +10311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>685</v>
       </c>
@@ -10250,7 +10329,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="334" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>687</v>
       </c>
@@ -10265,7 +10344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>689</v>
       </c>
@@ -10280,7 +10359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>692</v>
       </c>
@@ -10298,7 +10377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>693</v>
       </c>
@@ -10316,7 +10395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>695</v>
       </c>
@@ -10334,7 +10413,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="339" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>698</v>
       </c>
@@ -10349,7 +10428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>699</v>
       </c>
@@ -10370,7 +10449,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="341" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>702</v>
       </c>
@@ -10385,7 +10464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>704</v>
       </c>
@@ -10400,7 +10479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>705</v>
       </c>
@@ -10415,7 +10494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>708</v>
       </c>
@@ -10430,7 +10509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>710</v>
       </c>
@@ -10448,7 +10527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="346" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>712</v>
       </c>
@@ -10466,7 +10545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>715</v>
       </c>
@@ -10487,7 +10566,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="348" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>718</v>
       </c>
@@ -10502,7 +10581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>720</v>
       </c>
@@ -10517,7 +10596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>722</v>
       </c>
@@ -10535,7 +10614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>724</v>
       </c>
@@ -10550,7 +10629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>725</v>
       </c>
@@ -10568,7 +10647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>726</v>
       </c>
@@ -10586,7 +10665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="354" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>727</v>
       </c>
@@ -10604,42 +10683,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="355" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A355" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R1">
-    <sortState ref="A2:R79">
+  <autoFilter ref="A1:R1" xr:uid="{00000000-0009-0000-0000-000006000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R79">
       <sortCondition descending="1" ref="O1"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:R308">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R308">
     <sortCondition descending="1" ref="O2:O308"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" display="mailto:jacksepticeye7@gmail.com"/>
-    <hyperlink ref="P3" r:id="rId2" display="mailto:markiplierbusiness@gmail.com"/>
-    <hyperlink ref="P83" r:id="rId3" display="http://www.afromask.com/afro0mask@gmail.com"/>
-    <hyperlink ref="P25" r:id="rId4"/>
-    <hyperlink ref="P26" r:id="rId5"/>
-    <hyperlink ref="P32" r:id="rId6"/>
-    <hyperlink ref="P85" r:id="rId7"/>
-    <hyperlink ref="P62" r:id="rId8"/>
-    <hyperlink ref="P112" r:id="rId9"/>
-    <hyperlink ref="P126" r:id="rId10"/>
-    <hyperlink ref="P142" r:id="rId11"/>
-    <hyperlink ref="R27" r:id="rId12"/>
-    <hyperlink ref="P157" r:id="rId13"/>
-    <hyperlink ref="P48" r:id="rId14"/>
-    <hyperlink ref="P59" r:id="rId15"/>
-    <hyperlink ref="P94" r:id="rId16"/>
-    <hyperlink ref="P95" r:id="rId17"/>
-    <hyperlink ref="P114" r:id="rId18"/>
-    <hyperlink ref="P51" r:id="rId19"/>
-    <hyperlink ref="P55" r:id="rId20" display="mailto:gilathiss.biznes@gmail.com"/>
-    <hyperlink ref="P133" r:id="rId21"/>
-    <hyperlink ref="P322" r:id="rId22" display="mailto:jpad17officialchannel@gmail.com"/>
-    <hyperlink ref="P342" r:id="rId23"/>
+    <hyperlink ref="P2" r:id="rId1" display="mailto:jacksepticeye7@gmail.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="P3" r:id="rId2" display="mailto:markiplierbusiness@gmail.com" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="P83" r:id="rId3" display="http://www.afromask.com/afro0mask@gmail.com" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="P25" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="P26" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="P32" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="P85" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="P62" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="P112" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="P126" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
+    <hyperlink ref="P142" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
+    <hyperlink ref="R27" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
+    <hyperlink ref="P157" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
+    <hyperlink ref="P48" r:id="rId14" xr:uid="{00000000-0004-0000-0600-00000D000000}"/>
+    <hyperlink ref="P59" r:id="rId15" xr:uid="{00000000-0004-0000-0600-00000E000000}"/>
+    <hyperlink ref="P94" r:id="rId16" xr:uid="{00000000-0004-0000-0600-00000F000000}"/>
+    <hyperlink ref="P95" r:id="rId17" xr:uid="{00000000-0004-0000-0600-000010000000}"/>
+    <hyperlink ref="P114" r:id="rId18" xr:uid="{00000000-0004-0000-0600-000011000000}"/>
+    <hyperlink ref="P51" r:id="rId19" xr:uid="{00000000-0004-0000-0600-000012000000}"/>
+    <hyperlink ref="P55" r:id="rId20" display="mailto:gilathiss.biznes@gmail.com" xr:uid="{00000000-0004-0000-0600-000013000000}"/>
+    <hyperlink ref="P133" r:id="rId21" xr:uid="{00000000-0004-0000-0600-000014000000}"/>
+    <hyperlink ref="P322" r:id="rId22" display="mailto:jpad17officialchannel@gmail.com" xr:uid="{00000000-0004-0000-0600-000015000000}"/>
+    <hyperlink ref="P342" r:id="rId23" xr:uid="{00000000-0004-0000-0600-000016000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId24"/>
@@ -10647,32 +10726,32 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>735</v>
       </c>
@@ -10680,32 +10759,32 @@
         <v>736</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>742</v>
       </c>
@@ -10715,33 +10794,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
Small updating to planning file
</commit_message>
<xml_diff>
--- a/Marketing planning.xlsx
+++ b/Marketing planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wstoop\Documents\thesapling-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12DAA39-5DC1-4112-844D-5DD985DC4B34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6074F032-41EE-4AB5-AABE-E0666B4BA298}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overzicht" sheetId="1" r:id="rId1"/>
@@ -4458,8 +4458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4553,8 +4553,8 @@
       <c r="F4" t="s">
         <v>755</v>
       </c>
-      <c r="G4" t="s">
-        <v>523</v>
+      <c r="G4" s="19" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -4981,7 +4981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U360"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="I280" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Second batch of youtubers
</commit_message>
<xml_diff>
--- a/Marketing planning.xlsx
+++ b/Marketing planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wstoop\Documents\thesapling-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CE9983-5F3F-4B81-BE5C-209842073511}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DC5DE7-54FD-4ABA-B9A0-CECB7D205C98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overzicht" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="905">
   <si>
     <t>Week</t>
   </si>
@@ -2774,6 +2774,15 @@
   </si>
   <si>
     <t>My Spore-inspired ecology sim: now with flowers and bioluminescence</t>
+  </si>
+  <si>
+    <t>Reactie</t>
+  </si>
+  <si>
+    <t>aardig, maar niet actief</t>
+  </si>
+  <si>
+    <t>gamedev</t>
   </si>
 </sst>
 </file>
@@ -3717,7 +3726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -4989,13 +4998,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:U360"/>
+  <dimension ref="A1:V360"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I280" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B305" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R296" sqref="R296"/>
+      <selection pane="bottomRight" activeCell="A317" sqref="A317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5016,7 +5025,7 @@
     <col min="18" max="18" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>158</v>
       </c>
@@ -5080,8 +5089,11 @@
       <c r="U1" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V1" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>169</v>
       </c>
@@ -5106,7 +5118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -5131,7 +5143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -5159,7 +5171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>167</v>
       </c>
@@ -5187,7 +5199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>352</v>
       </c>
@@ -5209,7 +5221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>409</v>
       </c>
@@ -5231,7 +5243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>227</v>
       </c>
@@ -5253,7 +5265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>202</v>
       </c>
@@ -5275,7 +5287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>176</v>
       </c>
@@ -5297,7 +5309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>360</v>
       </c>
@@ -5319,7 +5331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>366</v>
       </c>
@@ -5341,7 +5353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>365</v>
       </c>
@@ -5363,7 +5375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>354</v>
       </c>
@@ -5382,7 +5394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>345</v>
       </c>
@@ -5404,7 +5416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>286</v>
       </c>
@@ -7613,7 +7625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>228</v>
       </c>
@@ -7635,7 +7647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>279</v>
       </c>
@@ -7659,8 +7671,11 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V114" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="115" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>420</v>
       </c>
@@ -7682,7 +7697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>216</v>
       </c>
@@ -7704,7 +7719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>242</v>
       </c>
@@ -7729,7 +7744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>247</v>
       </c>
@@ -7751,7 +7766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>103</v>
       </c>
@@ -7776,7 +7791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>181</v>
       </c>
@@ -7798,7 +7813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>230</v>
       </c>
@@ -7820,7 +7835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>195</v>
       </c>
@@ -7839,7 +7854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>106</v>
       </c>
@@ -7861,7 +7876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>299</v>
       </c>
@@ -7880,7 +7895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>229</v>
       </c>
@@ -7905,7 +7920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>123</v>
       </c>
@@ -7927,7 +7942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>290</v>
       </c>
@@ -7946,7 +7961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>397</v>
       </c>
@@ -11628,7 +11643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>687</v>
       </c>
@@ -11646,7 +11661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>689</v>
       </c>
@@ -11664,7 +11679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="339" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>692</v>
       </c>
@@ -11679,7 +11694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>693</v>
       </c>
@@ -11700,7 +11715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="341" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>696</v>
       </c>
@@ -11715,7 +11730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>698</v>
       </c>
@@ -11730,7 +11745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>699</v>
       </c>
@@ -11745,7 +11760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>702</v>
       </c>
@@ -11760,7 +11775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>704</v>
       </c>
@@ -11778,7 +11793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="346" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>706</v>
       </c>
@@ -11796,7 +11811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>709</v>
       </c>
@@ -11816,8 +11831,11 @@
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="348" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V347" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="348" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>712</v>
       </c>
@@ -11832,7 +11850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>714</v>
       </c>
@@ -11847,7 +11865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>716</v>
       </c>
@@ -11865,7 +11883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>718</v>
       </c>
@@ -11880,7 +11898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>719</v>
       </c>

</xml_diff>

<commit_message>
Processed email in marketing planning
</commit_message>
<xml_diff>
--- a/Marketing planning.xlsx
+++ b/Marketing planning.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wstoop\Documents\thesapling-website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wessel\Desktop\thesapling-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DC5DE7-54FD-4ABA-B9A0-CECB7D205C98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="782" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Overzicht" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Filmpjesmakers!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Nieuwe Youtubers'!$A$1:$T$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="907">
   <si>
     <t>Week</t>
   </si>
@@ -2784,11 +2783,17 @@
   <si>
     <t>gamedev</t>
   </si>
+  <si>
+    <t>interested</t>
+  </si>
+  <si>
+    <t>raar engels, positef</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2945,7 +2950,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3256,7 +3261,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3266,20 +3271,20 @@
       <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="20.5546875" style="1"/>
-    <col min="8" max="8" width="20.5546875" style="1"/>
-    <col min="11" max="16" width="20.5546875" style="1"/>
-    <col min="17" max="17" width="11.33203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5546875" style="1"/>
-    <col min="21" max="16384" width="20.5546875" style="1"/>
+    <col min="1" max="1" width="14.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="20.5703125" style="1"/>
+    <col min="8" max="8" width="20.5703125" style="1"/>
+    <col min="11" max="16" width="20.5703125" style="1"/>
+    <col min="17" max="17" width="11.28515625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="20.5703125" style="1"/>
+    <col min="21" max="16384" width="20.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="6" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
@@ -3344,7 +3349,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>38</v>
       </c>
@@ -3361,7 +3366,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>39</v>
       </c>
@@ -3380,7 +3385,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>40</v>
       </c>
@@ -3399,7 +3404,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>41</v>
       </c>
@@ -3421,7 +3426,7 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>42</v>
       </c>
@@ -3440,7 +3445,7 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>43</v>
       </c>
@@ -3459,7 +3464,7 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>44</v>
       </c>
@@ -3481,7 +3486,7 @@
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:21" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>45</v>
       </c>
@@ -3537,7 +3542,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>46</v>
       </c>
@@ -3562,7 +3567,7 @@
       <c r="J10" s="1"/>
       <c r="K10"/>
     </row>
-    <row r="11" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>47</v>
       </c>
@@ -3587,7 +3592,7 @@
       <c r="J11" s="1"/>
       <c r="K11"/>
     </row>
-    <row r="12" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>48</v>
       </c>
@@ -3612,7 +3617,7 @@
       <c r="J12" s="1"/>
       <c r="K12"/>
     </row>
-    <row r="13" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>49</v>
       </c>
@@ -3640,7 +3645,7 @@
       <c r="J13" s="1"/>
       <c r="K13"/>
     </row>
-    <row r="14" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>50</v>
       </c>
@@ -3696,7 +3701,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -3723,20 +3728,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>738</v>
       </c>
@@ -3750,7 +3755,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -3764,7 +3769,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>874</v>
       </c>
@@ -3778,7 +3783,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>873</v>
       </c>
@@ -3792,7 +3797,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>874</v>
       </c>
@@ -3812,25 +3817,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -3844,7 +3849,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -3858,7 +3863,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>870</v>
       </c>
@@ -3866,7 +3871,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -3880,19 +3885,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>818</v>
       </c>
@@ -3903,7 +3908,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>819</v>
       </c>
@@ -3914,7 +3919,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>820</v>
       </c>
@@ -3925,7 +3930,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>821</v>
       </c>
@@ -3936,7 +3941,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>822</v>
       </c>
@@ -3947,7 +3952,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>823</v>
       </c>
@@ -3958,7 +3963,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>824</v>
       </c>
@@ -3969,7 +3974,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>804</v>
       </c>
@@ -3980,7 +3985,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>825</v>
       </c>
@@ -3991,7 +3996,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>826</v>
       </c>
@@ -4002,7 +4007,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>827</v>
       </c>
@@ -4013,7 +4018,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>828</v>
       </c>
@@ -4024,7 +4029,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>829</v>
       </c>
@@ -4035,7 +4040,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>830</v>
       </c>
@@ -4046,7 +4051,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>831</v>
       </c>
@@ -4057,7 +4062,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>832</v>
       </c>
@@ -4068,7 +4073,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>833</v>
       </c>
@@ -4079,7 +4084,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>837</v>
       </c>
@@ -4090,7 +4095,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>836</v>
       </c>
@@ -4101,7 +4106,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>854</v>
       </c>
@@ -4112,7 +4117,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>898</v>
       </c>
@@ -4125,29 +4130,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C18" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="C19" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="C21" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C18" r:id="rId1"/>
+    <hyperlink ref="C19" r:id="rId2"/>
+    <hyperlink ref="C21" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5546875" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>838</v>
       </c>
@@ -4155,7 +4160,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>839</v>
       </c>
@@ -4163,7 +4168,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>840</v>
       </c>
@@ -4171,7 +4176,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>841</v>
       </c>
@@ -4179,7 +4184,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>900</v>
       </c>
@@ -4187,7 +4192,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>842</v>
       </c>
@@ -4195,7 +4200,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>843</v>
       </c>
@@ -4205,23 +4210,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>774</v>
       </c>
@@ -4232,7 +4237,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>776</v>
       </c>
@@ -4243,7 +4248,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>778</v>
       </c>
@@ -4254,7 +4259,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>780</v>
       </c>
@@ -4265,7 +4270,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>782</v>
       </c>
@@ -4276,7 +4281,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>784</v>
       </c>
@@ -4287,7 +4292,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>478</v>
       </c>
@@ -4298,7 +4303,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>787</v>
       </c>
@@ -4309,7 +4314,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>789</v>
       </c>
@@ -4320,7 +4325,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>791</v>
       </c>
@@ -4331,7 +4336,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>571</v>
       </c>
@@ -4342,7 +4347,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>794</v>
       </c>
@@ -4353,7 +4358,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>478</v>
       </c>
@@ -4364,7 +4369,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>797</v>
       </c>
@@ -4375,7 +4380,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>799</v>
       </c>
@@ -4386,7 +4391,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>801</v>
       </c>
@@ -4397,7 +4402,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>803</v>
       </c>
@@ -4408,7 +4413,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>806</v>
       </c>
@@ -4419,7 +4424,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>851</v>
       </c>
@@ -4430,7 +4435,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>855</v>
       </c>
@@ -4441,7 +4446,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>857</v>
       </c>
@@ -4452,7 +4457,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>859</v>
       </c>
@@ -4465,8 +4470,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C19" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="C21" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C19" r:id="rId1"/>
+    <hyperlink ref="C21" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
@@ -4474,20 +4479,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>99</v>
       </c>
@@ -4513,7 +4518,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -4533,7 +4538,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -4556,7 +4561,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -4576,7 +4581,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -4596,7 +4601,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -4619,7 +4624,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -4636,7 +4641,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -4659,7 +4664,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>97</v>
       </c>
@@ -4676,7 +4681,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -4699,7 +4704,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -4716,7 +4721,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -4733,7 +4738,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>90</v>
       </c>
@@ -4750,7 +4755,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -4767,7 +4772,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>92</v>
       </c>
@@ -4784,7 +4789,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -4807,7 +4812,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>98</v>
       </c>
@@ -4824,7 +4829,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>327</v>
       </c>
@@ -4848,8 +4853,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000004000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D17">
+  <autoFilter ref="A1:D1">
+    <sortState ref="A2:D17">
       <sortCondition descending="1" ref="B1"/>
     </sortState>
   </autoFilter>
@@ -4859,134 +4864,134 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>344</v>
       </c>
@@ -4997,35 +5002,35 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V360"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B305" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A317" sqref="A317"/>
+      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
     <col min="13" max="15" width="21" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
-    <col min="17" max="17" width="9.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.33203125" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>158</v>
       </c>
@@ -5093,7 +5098,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>169</v>
       </c>
@@ -5118,7 +5123,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -5143,7 +5148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -5171,7 +5176,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>167</v>
       </c>
@@ -5199,7 +5204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>352</v>
       </c>
@@ -5220,8 +5225,11 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="V6" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>409</v>
       </c>
@@ -5243,7 +5251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>227</v>
       </c>
@@ -5265,7 +5273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>202</v>
       </c>
@@ -5287,7 +5295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>176</v>
       </c>
@@ -5309,7 +5317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>360</v>
       </c>
@@ -5331,7 +5339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>366</v>
       </c>
@@ -5353,7 +5361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>365</v>
       </c>
@@ -5375,7 +5383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>354</v>
       </c>
@@ -5394,7 +5402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>345</v>
       </c>
@@ -5416,7 +5424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>286</v>
       </c>
@@ -5441,7 +5449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>349</v>
       </c>
@@ -5469,7 +5477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>115</v>
       </c>
@@ -5491,7 +5499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>355</v>
       </c>
@@ -5513,7 +5521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>369</v>
       </c>
@@ -5532,7 +5540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>308</v>
       </c>
@@ -5551,7 +5559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>251</v>
       </c>
@@ -5576,7 +5584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>393</v>
       </c>
@@ -5592,7 +5600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>313</v>
       </c>
@@ -5617,7 +5625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>126</v>
       </c>
@@ -5639,7 +5647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>243</v>
       </c>
@@ -5667,7 +5675,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>172</v>
       </c>
@@ -5692,7 +5700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>350</v>
       </c>
@@ -5714,7 +5722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>182</v>
       </c>
@@ -5736,7 +5744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>187</v>
       </c>
@@ -5755,7 +5763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>221</v>
       </c>
@@ -5777,7 +5785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>131</v>
       </c>
@@ -5796,7 +5804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>173</v>
       </c>
@@ -5818,7 +5826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>282</v>
       </c>
@@ -5843,7 +5851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>348</v>
       </c>
@@ -5868,7 +5876,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>252</v>
       </c>
@@ -5896,7 +5904,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>287</v>
       </c>
@@ -5921,7 +5929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>190</v>
       </c>
@@ -5943,7 +5951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>284</v>
       </c>
@@ -5965,7 +5973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>239</v>
       </c>
@@ -5993,7 +6001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>183</v>
       </c>
@@ -6018,7 +6026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>170</v>
       </c>
@@ -6043,7 +6051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>201</v>
       </c>
@@ -6065,7 +6073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>519</v>
       </c>
@@ -6087,7 +6095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>110</v>
       </c>
@@ -6112,7 +6120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>253</v>
       </c>
@@ -6131,7 +6139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>259</v>
       </c>
@@ -6150,7 +6158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>269</v>
       </c>
@@ -6178,7 +6186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>171</v>
       </c>
@@ -6200,7 +6208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>235</v>
       </c>
@@ -6225,7 +6233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>395</v>
       </c>
@@ -6244,7 +6252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>254</v>
       </c>
@@ -6266,7 +6274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -6288,7 +6296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>417</v>
       </c>
@@ -6310,7 +6318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>346</v>
       </c>
@@ -6329,7 +6337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>358</v>
       </c>
@@ -6357,7 +6365,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>189</v>
       </c>
@@ -6376,7 +6384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>226</v>
       </c>
@@ -6401,7 +6409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>175</v>
       </c>
@@ -6423,7 +6431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>361</v>
       </c>
@@ -6448,7 +6456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>359</v>
       </c>
@@ -6470,7 +6478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>204</v>
       </c>
@@ -6495,7 +6503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>112</v>
       </c>
@@ -6529,7 +6537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>389</v>
       </c>
@@ -6554,7 +6562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>261</v>
       </c>
@@ -6579,7 +6587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>233</v>
       </c>
@@ -6598,7 +6606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>237</v>
       </c>
@@ -6617,7 +6625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>428</v>
       </c>
@@ -6639,7 +6647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>213</v>
       </c>
@@ -6658,7 +6666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>294</v>
       </c>
@@ -6686,7 +6694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>382</v>
       </c>
@@ -6714,7 +6722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>310</v>
       </c>
@@ -6736,7 +6744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>271</v>
       </c>
@@ -6758,7 +6766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>191</v>
       </c>
@@ -6779,8 +6787,11 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V74" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>278</v>
       </c>
@@ -6799,7 +6810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>174</v>
       </c>
@@ -6827,7 +6838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>164</v>
       </c>
@@ -6846,7 +6857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>178</v>
       </c>
@@ -6868,7 +6879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>285</v>
       </c>
@@ -6896,7 +6907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>177</v>
       </c>
@@ -6921,7 +6932,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>277</v>
       </c>
@@ -6940,7 +6951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>136</v>
       </c>
@@ -6959,7 +6970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>206</v>
       </c>
@@ -6984,7 +6995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>101</v>
       </c>
@@ -7006,7 +7017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>128</v>
       </c>
@@ -7028,7 +7039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>218</v>
       </c>
@@ -7047,7 +7058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>267</v>
       </c>
@@ -7066,7 +7077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>380</v>
       </c>
@@ -7085,7 +7096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>194</v>
       </c>
@@ -7110,7 +7121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>193</v>
       </c>
@@ -7132,7 +7143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>196</v>
       </c>
@@ -7157,7 +7168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>272</v>
       </c>
@@ -7182,7 +7193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>166</v>
       </c>
@@ -7201,7 +7212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>185</v>
       </c>
@@ -7220,7 +7231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>184</v>
       </c>
@@ -7242,7 +7253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>362</v>
       </c>
@@ -7261,7 +7272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>413</v>
       </c>
@@ -7286,7 +7297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>225</v>
       </c>
@@ -7305,7 +7316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>356</v>
       </c>
@@ -7327,7 +7338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>192</v>
       </c>
@@ -7352,7 +7363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>402</v>
       </c>
@@ -7374,7 +7385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>215</v>
       </c>
@@ -7393,7 +7404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>222</v>
       </c>
@@ -7421,7 +7432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>248</v>
       </c>
@@ -7440,7 +7451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>398</v>
       </c>
@@ -7462,7 +7473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>207</v>
       </c>
@@ -7481,7 +7492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>255</v>
       </c>
@@ -7503,7 +7514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>353</v>
       </c>
@@ -7528,7 +7539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>224</v>
       </c>
@@ -7550,7 +7561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>199</v>
       </c>
@@ -7575,7 +7586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>127</v>
       </c>
@@ -7600,7 +7611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>205</v>
       </c>
@@ -7625,7 +7636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>228</v>
       </c>
@@ -7647,7 +7658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>279</v>
       </c>
@@ -7675,7 +7686,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>420</v>
       </c>
@@ -7697,7 +7708,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>216</v>
       </c>
@@ -7719,7 +7730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>242</v>
       </c>
@@ -7744,7 +7755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>247</v>
       </c>
@@ -7766,7 +7777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>103</v>
       </c>
@@ -7791,7 +7802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>181</v>
       </c>
@@ -7813,7 +7824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>230</v>
       </c>
@@ -7835,7 +7846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>195</v>
       </c>
@@ -7854,7 +7865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>106</v>
       </c>
@@ -7876,7 +7887,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>299</v>
       </c>
@@ -7895,7 +7906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>229</v>
       </c>
@@ -7920,7 +7931,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>123</v>
       </c>
@@ -7942,7 +7953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>290</v>
       </c>
@@ -7961,7 +7972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>397</v>
       </c>
@@ -7980,7 +7991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>258</v>
       </c>
@@ -8002,7 +8013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>423</v>
       </c>
@@ -8021,7 +8032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>240</v>
       </c>
@@ -8043,7 +8054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>315</v>
       </c>
@@ -8065,7 +8076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>401</v>
       </c>
@@ -8084,7 +8095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>179</v>
       </c>
@@ -8103,7 +8114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>208</v>
       </c>
@@ -8122,7 +8133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>351</v>
       </c>
@@ -8144,7 +8155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>121</v>
       </c>
@@ -8169,7 +8180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>214</v>
       </c>
@@ -8191,7 +8202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>118</v>
       </c>
@@ -8213,7 +8224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>198</v>
       </c>
@@ -8232,7 +8243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>107</v>
       </c>
@@ -8251,7 +8262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>125</v>
       </c>
@@ -8270,7 +8281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>135</v>
       </c>
@@ -8289,7 +8300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>211</v>
       </c>
@@ -8314,7 +8325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>223</v>
       </c>
@@ -8330,7 +8341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>266</v>
       </c>
@@ -8346,7 +8357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>105</v>
       </c>
@@ -8365,7 +8376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>347</v>
       </c>
@@ -8381,7 +8392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>408</v>
       </c>
@@ -8397,7 +8408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>108</v>
       </c>
@@ -8419,7 +8430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>262</v>
       </c>
@@ -8435,7 +8446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>311</v>
       </c>
@@ -8451,7 +8462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>145</v>
       </c>
@@ -8479,7 +8490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>377</v>
       </c>
@@ -8495,7 +8506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>317</v>
       </c>
@@ -8511,7 +8522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>160</v>
       </c>
@@ -8533,7 +8544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>113</v>
       </c>
@@ -8555,7 +8566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>263</v>
       </c>
@@ -8571,7 +8582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>399</v>
       </c>
@@ -8587,7 +8598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>250</v>
       </c>
@@ -8603,7 +8614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>273</v>
       </c>
@@ -8619,7 +8630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>268</v>
       </c>
@@ -8635,7 +8646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>367</v>
       </c>
@@ -8651,7 +8662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>186</v>
       </c>
@@ -8667,7 +8678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>244</v>
       </c>
@@ -8683,7 +8694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>390</v>
       </c>
@@ -8699,7 +8710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>119</v>
       </c>
@@ -8721,7 +8732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>165</v>
       </c>
@@ -8737,7 +8748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>238</v>
       </c>
@@ -8753,7 +8764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>302</v>
       </c>
@@ -8769,7 +8780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>120</v>
       </c>
@@ -8791,7 +8802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>117</v>
       </c>
@@ -8810,7 +8821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>180</v>
       </c>
@@ -8826,7 +8837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>197</v>
       </c>
@@ -8842,7 +8853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>280</v>
       </c>
@@ -8858,7 +8869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>281</v>
       </c>
@@ -8886,7 +8897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>134</v>
       </c>
@@ -8905,7 +8916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>188</v>
       </c>
@@ -8921,7 +8932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>291</v>
       </c>
@@ -8937,7 +8948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>292</v>
       </c>
@@ -8953,7 +8964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>406</v>
       </c>
@@ -8969,7 +8980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>210</v>
       </c>
@@ -8985,7 +8996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>220</v>
       </c>
@@ -9001,7 +9012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>383</v>
       </c>
@@ -9017,7 +9028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>425</v>
       </c>
@@ -9033,7 +9044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>133</v>
       </c>
@@ -9052,7 +9063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>312</v>
       </c>
@@ -9080,7 +9091,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>381</v>
       </c>
@@ -9096,7 +9107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>132</v>
       </c>
@@ -9115,7 +9126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>217</v>
       </c>
@@ -9131,7 +9142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>236</v>
       </c>
@@ -9147,7 +9158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>314</v>
       </c>
@@ -9163,7 +9174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>316</v>
       </c>
@@ -9179,7 +9190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>318</v>
       </c>
@@ -9195,7 +9206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>319</v>
       </c>
@@ -9211,7 +9222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>111</v>
       </c>
@@ -9233,7 +9244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>219</v>
       </c>
@@ -9255,7 +9266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>297</v>
       </c>
@@ -9271,7 +9282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>114</v>
       </c>
@@ -9293,7 +9304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>143</v>
       </c>
@@ -9315,7 +9326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>159</v>
       </c>
@@ -9334,7 +9345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>418</v>
       </c>
@@ -9350,7 +9361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>427</v>
       </c>
@@ -9366,7 +9377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>241</v>
       </c>
@@ -9382,7 +9393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>270</v>
       </c>
@@ -9398,7 +9409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>276</v>
       </c>
@@ -9414,7 +9425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>305</v>
       </c>
@@ -9430,7 +9441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>384</v>
       </c>
@@ -9446,7 +9457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>387</v>
       </c>
@@ -9462,7 +9473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>161</v>
       </c>
@@ -9487,7 +9498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="211" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>296</v>
       </c>
@@ -9503,7 +9514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>306</v>
       </c>
@@ -9519,7 +9530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>430</v>
       </c>
@@ -9535,7 +9546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>129</v>
       </c>
@@ -9560,7 +9571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>149</v>
       </c>
@@ -9576,7 +9587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>148</v>
       </c>
@@ -9592,7 +9603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>89</v>
       </c>
@@ -9608,7 +9619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>260</v>
       </c>
@@ -9624,7 +9635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>295</v>
       </c>
@@ -9640,7 +9651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>309</v>
       </c>
@@ -9656,7 +9667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>364</v>
       </c>
@@ -9672,7 +9683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>376</v>
       </c>
@@ -9688,7 +9699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>391</v>
       </c>
@@ -9704,7 +9715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>139</v>
       </c>
@@ -9720,7 +9731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>142</v>
       </c>
@@ -9736,7 +9747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>257</v>
       </c>
@@ -9752,7 +9763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>283</v>
       </c>
@@ -9768,7 +9779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>298</v>
       </c>
@@ -9784,7 +9795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>307</v>
       </c>
@@ -9800,7 +9811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>147</v>
       </c>
@@ -9816,7 +9827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>304</v>
       </c>
@@ -9832,7 +9843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>394</v>
       </c>
@@ -9848,7 +9859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>124</v>
       </c>
@@ -9864,7 +9875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>141</v>
       </c>
@@ -9880,7 +9891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>144</v>
       </c>
@@ -9896,7 +9907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>274</v>
       </c>
@@ -9912,7 +9923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>396</v>
       </c>
@@ -9928,7 +9939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>102</v>
       </c>
@@ -9944,7 +9955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>146</v>
       </c>
@@ -9969,7 +9980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="240" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>303</v>
       </c>
@@ -9985,7 +9996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>375</v>
       </c>
@@ -10001,7 +10012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>388</v>
       </c>
@@ -10017,7 +10028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>404</v>
       </c>
@@ -10033,7 +10044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>407</v>
       </c>
@@ -10058,7 +10069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>203</v>
       </c>
@@ -10074,7 +10085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>209</v>
       </c>
@@ -10090,7 +10101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>212</v>
       </c>
@@ -10106,7 +10117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>232</v>
       </c>
@@ -10122,7 +10133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>234</v>
       </c>
@@ -10138,7 +10149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -10154,7 +10165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>256</v>
       </c>
@@ -10170,7 +10181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>288</v>
       </c>
@@ -10186,7 +10197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>300</v>
       </c>
@@ -10202,7 +10213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>301</v>
       </c>
@@ -10218,7 +10229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>372</v>
       </c>
@@ -10234,7 +10245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>385</v>
       </c>
@@ -10250,7 +10261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>400</v>
       </c>
@@ -10266,7 +10277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>405</v>
       </c>
@@ -10282,7 +10293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>410</v>
       </c>
@@ -10298,7 +10309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>415</v>
       </c>
@@ -10314,7 +10325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>422</v>
       </c>
@@ -10330,7 +10341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>433</v>
       </c>
@@ -10346,7 +10357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>403</v>
       </c>
@@ -10362,7 +10373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>116</v>
       </c>
@@ -10378,7 +10389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>162</v>
       </c>
@@ -10394,7 +10405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>168</v>
       </c>
@@ -10410,7 +10421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>200</v>
       </c>
@@ -10426,7 +10437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>245</v>
       </c>
@@ -10442,7 +10453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>246</v>
       </c>
@@ -10458,7 +10469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>289</v>
       </c>
@@ -10474,7 +10485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>357</v>
       </c>
@@ -10490,7 +10501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>370</v>
       </c>
@@ -10506,7 +10517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>373</v>
       </c>
@@ -10522,7 +10533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>378</v>
       </c>
@@ -10538,7 +10549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>386</v>
       </c>
@@ -10554,7 +10565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>392</v>
       </c>
@@ -10570,7 +10581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>411</v>
       </c>
@@ -10586,7 +10597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>412</v>
       </c>
@@ -10602,7 +10613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>414</v>
       </c>
@@ -10618,7 +10629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>416</v>
       </c>
@@ -10634,7 +10645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>421</v>
       </c>
@@ -10650,7 +10661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>431</v>
       </c>
@@ -10666,7 +10677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>432</v>
       </c>
@@ -10682,7 +10693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>435</v>
       </c>
@@ -10698,7 +10709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>436</v>
       </c>
@@ -10714,7 +10725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>437</v>
       </c>
@@ -10730,7 +10741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>109</v>
       </c>
@@ -10746,7 +10757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>130</v>
       </c>
@@ -10762,7 +10773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>137</v>
       </c>
@@ -10778,7 +10789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>138</v>
       </c>
@@ -10794,7 +10805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>140</v>
       </c>
@@ -10810,7 +10821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>264</v>
       </c>
@@ -10826,7 +10837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>265</v>
       </c>
@@ -10842,7 +10853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>275</v>
       </c>
@@ -10858,7 +10869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>293</v>
       </c>
@@ -10874,7 +10885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>892</v>
       </c>
@@ -10896,7 +10907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>363</v>
       </c>
@@ -10912,7 +10923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>368</v>
       </c>
@@ -10928,7 +10939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>371</v>
       </c>
@@ -10944,7 +10955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>374</v>
       </c>
@@ -10960,7 +10971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>379</v>
       </c>
@@ -10976,7 +10987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>419</v>
       </c>
@@ -10992,7 +11003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>424</v>
       </c>
@@ -11008,7 +11019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>426</v>
       </c>
@@ -11024,7 +11035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>429</v>
       </c>
@@ -11040,7 +11051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>434</v>
       </c>
@@ -11056,7 +11067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>163</v>
       </c>
@@ -11072,7 +11083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>625</v>
       </c>
@@ -11091,7 +11102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>626</v>
       </c>
@@ -11110,7 +11121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>628</v>
       </c>
@@ -11132,7 +11143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="311" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>631</v>
       </c>
@@ -11154,7 +11165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>633</v>
       </c>
@@ -11176,7 +11187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>636</v>
       </c>
@@ -11201,7 +11212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="314" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>641</v>
       </c>
@@ -11223,7 +11234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>642</v>
       </c>
@@ -11242,7 +11253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>644</v>
       </c>
@@ -11267,7 +11278,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="317" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>646</v>
       </c>
@@ -11289,7 +11300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>648</v>
       </c>
@@ -11314,7 +11325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="319" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>650</v>
       </c>
@@ -11339,7 +11350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="320" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>652</v>
       </c>
@@ -11358,7 +11369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>654</v>
       </c>
@@ -11377,7 +11388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>656</v>
       </c>
@@ -11396,7 +11407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>658</v>
       </c>
@@ -11418,7 +11429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>659</v>
       </c>
@@ -11437,7 +11448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>661</v>
       </c>
@@ -11459,7 +11470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="326" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>663</v>
       </c>
@@ -11481,7 +11492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>666</v>
       </c>
@@ -11496,7 +11507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>668</v>
       </c>
@@ -11511,7 +11522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>670</v>
       </c>
@@ -11529,7 +11540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>673</v>
       </c>
@@ -11544,7 +11555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>675</v>
       </c>
@@ -11562,7 +11573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="332" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>677</v>
       </c>
@@ -11577,7 +11588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>679</v>
       </c>
@@ -11595,7 +11606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="334" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>681</v>
       </c>
@@ -11610,7 +11621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>683</v>
       </c>
@@ -11625,7 +11636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>686</v>
       </c>
@@ -11643,7 +11654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>687</v>
       </c>
@@ -11661,7 +11672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>689</v>
       </c>
@@ -11679,7 +11690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="339" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>692</v>
       </c>
@@ -11694,7 +11705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>693</v>
       </c>
@@ -11715,7 +11726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="341" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>696</v>
       </c>
@@ -11730,7 +11741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>698</v>
       </c>
@@ -11745,7 +11756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>699</v>
       </c>
@@ -11760,7 +11771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>702</v>
       </c>
@@ -11775,7 +11786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>704</v>
       </c>
@@ -11793,7 +11804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="346" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>706</v>
       </c>
@@ -11811,7 +11822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>709</v>
       </c>
@@ -11835,7 +11846,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="348" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>712</v>
       </c>
@@ -11850,7 +11861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>714</v>
       </c>
@@ -11865,7 +11876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>716</v>
       </c>
@@ -11883,7 +11894,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="351" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>718</v>
       </c>
@@ -11898,7 +11909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>719</v>
       </c>
@@ -11916,7 +11927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>720</v>
       </c>
@@ -11934,7 +11945,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="354" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>721</v>
       </c>
@@ -11952,7 +11963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="355" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A355" s="17" t="s">
         <v>880</v>
       </c>
@@ -11966,7 +11977,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="356" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>881</v>
       </c>
@@ -11977,7 +11988,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="357" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>885</v>
       </c>
@@ -11994,7 +12005,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="358" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>887</v>
       </c>
@@ -12008,7 +12019,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="359" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>888</v>
       </c>
@@ -12025,7 +12036,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="360" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>236</v>
       </c>
@@ -12043,38 +12054,38 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T1" xr:uid="{00000000-0009-0000-0000-000006000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T79">
+  <autoFilter ref="A1:T1">
+    <sortState ref="A2:T79">
       <sortCondition descending="1" ref="Q1"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T308">
+  <sortState ref="A2:T308">
     <sortCondition descending="1" ref="Q2:Q308"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="R2" r:id="rId1" display="mailto:jacksepticeye7@gmail.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="R3" r:id="rId2" display="mailto:markiplierbusiness@gmail.com" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="R83" r:id="rId3" display="http://www.afromask.com/afro0mask@gmail.com" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="R25" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
-    <hyperlink ref="R26" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
-    <hyperlink ref="R32" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
-    <hyperlink ref="R85" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
-    <hyperlink ref="R62" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
-    <hyperlink ref="R112" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
-    <hyperlink ref="R126" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
-    <hyperlink ref="R142" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
-    <hyperlink ref="T27" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
-    <hyperlink ref="R157" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
-    <hyperlink ref="R48" r:id="rId14" xr:uid="{00000000-0004-0000-0600-00000D000000}"/>
-    <hyperlink ref="R59" r:id="rId15" xr:uid="{00000000-0004-0000-0600-00000E000000}"/>
-    <hyperlink ref="R94" r:id="rId16" xr:uid="{00000000-0004-0000-0600-00000F000000}"/>
-    <hyperlink ref="R95" r:id="rId17" xr:uid="{00000000-0004-0000-0600-000010000000}"/>
-    <hyperlink ref="R114" r:id="rId18" xr:uid="{00000000-0004-0000-0600-000011000000}"/>
-    <hyperlink ref="R51" r:id="rId19" xr:uid="{00000000-0004-0000-0600-000012000000}"/>
-    <hyperlink ref="R55" r:id="rId20" display="mailto:gilathiss.biznes@gmail.com" xr:uid="{00000000-0004-0000-0600-000013000000}"/>
-    <hyperlink ref="R133" r:id="rId21" xr:uid="{00000000-0004-0000-0600-000014000000}"/>
-    <hyperlink ref="R322" r:id="rId22" display="mailto:jpad17officialchannel@gmail.com" xr:uid="{00000000-0004-0000-0600-000015000000}"/>
-    <hyperlink ref="R342" r:id="rId23" xr:uid="{00000000-0004-0000-0600-000016000000}"/>
+    <hyperlink ref="R2" r:id="rId1" display="mailto:jacksepticeye7@gmail.com"/>
+    <hyperlink ref="R3" r:id="rId2" display="mailto:markiplierbusiness@gmail.com"/>
+    <hyperlink ref="R83" r:id="rId3" display="http://www.afromask.com/afro0mask@gmail.com"/>
+    <hyperlink ref="R25" r:id="rId4"/>
+    <hyperlink ref="R26" r:id="rId5"/>
+    <hyperlink ref="R32" r:id="rId6"/>
+    <hyperlink ref="R85" r:id="rId7"/>
+    <hyperlink ref="R62" r:id="rId8"/>
+    <hyperlink ref="R112" r:id="rId9"/>
+    <hyperlink ref="R126" r:id="rId10"/>
+    <hyperlink ref="R142" r:id="rId11"/>
+    <hyperlink ref="T27" r:id="rId12"/>
+    <hyperlink ref="R157" r:id="rId13"/>
+    <hyperlink ref="R48" r:id="rId14"/>
+    <hyperlink ref="R59" r:id="rId15"/>
+    <hyperlink ref="R94" r:id="rId16"/>
+    <hyperlink ref="R95" r:id="rId17"/>
+    <hyperlink ref="R114" r:id="rId18"/>
+    <hyperlink ref="R51" r:id="rId19"/>
+    <hyperlink ref="R55" r:id="rId20" display="mailto:gilathiss.biznes@gmail.com"/>
+    <hyperlink ref="R133" r:id="rId21"/>
+    <hyperlink ref="R322" r:id="rId22" display="mailto:jpad17officialchannel@gmail.com"/>
+    <hyperlink ref="R342" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId24"/>
@@ -12082,33 +12093,33 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>729</v>
       </c>
@@ -12116,32 +12127,32 @@
         <v>730</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>736</v>
       </c>
@@ -12149,12 +12160,12 @@
         <v>737</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>764</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>876</v>
       </c>
@@ -12167,26 +12178,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>872</v>
       </c>
@@ -12200,7 +12211,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -12214,12 +12225,12 @@
         <v>867</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
Added Adapt dev info
</commit_message>
<xml_diff>
--- a/Marketing planning.xlsx
+++ b/Marketing planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wstoop\Documents\thesapling-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E33D9F-E793-42EB-BAC7-8CB0EAAF2DF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2526023-174E-4C65-ADE7-379B676D4C13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overzicht" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="920">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="922">
   <si>
     <t>Week</t>
   </si>
@@ -2251,9 +2251,6 @@
     <t>Sheepdog</t>
   </si>
   <si>
-    <t>RocketShip Studios?</t>
-  </si>
-  <si>
     <t>Dream storm studios?</t>
   </si>
   <si>
@@ -2828,6 +2825,15 @@
   </si>
   <si>
     <t>alexeidrummond</t>
+  </si>
+  <si>
+    <t>indiegaming</t>
+  </si>
+  <si>
+    <t>Makers van Adapt</t>
+  </si>
+  <si>
+    <t>RocketShip Studios / Paul Herve</t>
   </si>
 </sst>
 </file>
@@ -3772,7 +3778,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3783,16 +3789,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B1">
         <v>21000</v>
       </c>
       <c r="C1" t="s">
+        <v>861</v>
+      </c>
+      <c r="D1" t="s">
         <v>862</v>
-      </c>
-      <c r="D1" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3803,52 +3809,52 @@
         <v>500</v>
       </c>
       <c r="C2" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D2" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B3">
         <v>1000</v>
       </c>
       <c r="C3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B4">
         <v>1000</v>
       </c>
       <c r="C4" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D4" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>874</v>
+        <v>919</v>
       </c>
       <c r="B5">
         <v>1800</v>
       </c>
       <c r="C5" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D5" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
   </sheetData>
@@ -3872,7 +3878,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3883,10 +3889,10 @@
         <v>400</v>
       </c>
       <c r="C2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D2" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3897,15 +3903,15 @@
         <v>800</v>
       </c>
       <c r="C3" t="s">
+        <v>864</v>
+      </c>
+      <c r="D3" t="s">
         <v>865</v>
-      </c>
-      <c r="D3" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -3939,233 +3945,233 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B1" t="s">
+        <v>764</v>
+      </c>
+      <c r="C1" t="s">
         <v>765</v>
-      </c>
-      <c r="C1" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C3" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B4" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C4" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B5" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C5" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B6" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C6" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B7" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C7" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>803</v>
+      </c>
+      <c r="B8" t="s">
+        <v>764</v>
+      </c>
+      <c r="C8" t="s">
         <v>804</v>
-      </c>
-      <c r="B8" t="s">
-        <v>765</v>
-      </c>
-      <c r="C8" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B9" t="s">
+        <v>807</v>
+      </c>
+      <c r="C9" t="s">
         <v>808</v>
-      </c>
-      <c r="C9" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B10" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C10" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B11" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C11" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B12" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C12" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B13" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C13" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B14" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C14" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B15" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C15" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B16" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C16" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B17" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C17" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B18" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B19" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B20" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C20" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>897</v>
+      </c>
+      <c r="B21" t="s">
+        <v>764</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>898</v>
-      </c>
-      <c r="B21" t="s">
-        <v>765</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>899</v>
       </c>
     </row>
   </sheetData>
@@ -4194,58 +4200,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B2" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B5" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B6" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B7" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="B8" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
   </sheetData>
@@ -4268,68 +4274,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>773</v>
+      </c>
+      <c r="B1" t="s">
+        <v>764</v>
+      </c>
+      <c r="C1" t="s">
         <v>774</v>
-      </c>
-      <c r="B1" t="s">
-        <v>765</v>
-      </c>
-      <c r="C1" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>775</v>
+      </c>
+      <c r="B2" t="s">
+        <v>764</v>
+      </c>
+      <c r="C2" t="s">
         <v>776</v>
-      </c>
-      <c r="B2" t="s">
-        <v>765</v>
-      </c>
-      <c r="C2" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>777</v>
+      </c>
+      <c r="B3" t="s">
+        <v>764</v>
+      </c>
+      <c r="C3" t="s">
         <v>778</v>
-      </c>
-      <c r="B3" t="s">
-        <v>765</v>
-      </c>
-      <c r="C3" t="s">
-        <v>779</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>779</v>
+      </c>
+      <c r="B4" t="s">
+        <v>764</v>
+      </c>
+      <c r="C4" t="s">
         <v>780</v>
-      </c>
-      <c r="B4" t="s">
-        <v>765</v>
-      </c>
-      <c r="C4" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>781</v>
+      </c>
+      <c r="B5" t="s">
+        <v>764</v>
+      </c>
+      <c r="C5" t="s">
         <v>782</v>
-      </c>
-      <c r="B5" t="s">
-        <v>765</v>
-      </c>
-      <c r="C5" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>783</v>
+      </c>
+      <c r="B6" t="s">
+        <v>764</v>
+      </c>
+      <c r="C6" t="s">
         <v>784</v>
-      </c>
-      <c r="B6" t="s">
-        <v>765</v>
-      </c>
-      <c r="C6" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -4337,43 +4343,43 @@
         <v>478</v>
       </c>
       <c r="B7" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C7" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>786</v>
+      </c>
+      <c r="B8" t="s">
+        <v>764</v>
+      </c>
+      <c r="C8" t="s">
         <v>787</v>
-      </c>
-      <c r="B8" t="s">
-        <v>765</v>
-      </c>
-      <c r="C8" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>788</v>
+      </c>
+      <c r="B9" t="s">
+        <v>764</v>
+      </c>
+      <c r="C9" t="s">
         <v>789</v>
-      </c>
-      <c r="B9" t="s">
-        <v>765</v>
-      </c>
-      <c r="C9" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>790</v>
+      </c>
+      <c r="B10" t="s">
+        <v>764</v>
+      </c>
+      <c r="C10" t="s">
         <v>791</v>
-      </c>
-      <c r="B10" t="s">
-        <v>765</v>
-      </c>
-      <c r="C10" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -4381,21 +4387,21 @@
         <v>571</v>
       </c>
       <c r="B11" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C11" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>793</v>
+      </c>
+      <c r="B12" t="s">
+        <v>764</v>
+      </c>
+      <c r="C12" t="s">
         <v>794</v>
-      </c>
-      <c r="B12" t="s">
-        <v>765</v>
-      </c>
-      <c r="C12" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -4403,109 +4409,109 @@
         <v>478</v>
       </c>
       <c r="B13" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C13" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>796</v>
+      </c>
+      <c r="B14" t="s">
+        <v>764</v>
+      </c>
+      <c r="C14" t="s">
         <v>797</v>
-      </c>
-      <c r="B14" t="s">
-        <v>765</v>
-      </c>
-      <c r="C14" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>798</v>
+      </c>
+      <c r="B15" t="s">
+        <v>764</v>
+      </c>
+      <c r="C15" t="s">
         <v>799</v>
-      </c>
-      <c r="B15" t="s">
-        <v>765</v>
-      </c>
-      <c r="C15" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>800</v>
+      </c>
+      <c r="B16" t="s">
+        <v>764</v>
+      </c>
+      <c r="C16" t="s">
         <v>801</v>
-      </c>
-      <c r="B16" t="s">
-        <v>765</v>
-      </c>
-      <c r="C16" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="B17" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C17" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>805</v>
+      </c>
+      <c r="B18" t="s">
+        <v>764</v>
+      </c>
+      <c r="C18" t="s">
         <v>806</v>
-      </c>
-      <c r="B18" t="s">
-        <v>765</v>
-      </c>
-      <c r="C18" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>850</v>
+      </c>
+      <c r="B19" t="s">
+        <v>764</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>851</v>
-      </c>
-      <c r="B19" t="s">
-        <v>765</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>854</v>
+      </c>
+      <c r="B20" t="s">
+        <v>764</v>
+      </c>
+      <c r="C20" t="s">
         <v>855</v>
-      </c>
-      <c r="B20" t="s">
-        <v>765</v>
-      </c>
-      <c r="C20" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>856</v>
+      </c>
+      <c r="B21" t="s">
+        <v>764</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>857</v>
-      </c>
-      <c r="B21" t="s">
-        <v>765</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>858</v>
+      </c>
+      <c r="B22" t="s">
+        <v>807</v>
+      </c>
+      <c r="C22" t="s">
         <v>859</v>
-      </c>
-      <c r="B22" t="s">
-        <v>808</v>
-      </c>
-      <c r="C22" t="s">
-        <v>860</v>
       </c>
     </row>
   </sheetData>
@@ -4546,16 +4552,16 @@
         <v>95</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F1" s="18" t="s">
+        <v>750</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>751</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>752</v>
-      </c>
       <c r="H1" s="18" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -4569,10 +4575,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="F2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G2" t="s">
         <v>523</v>
@@ -4589,16 +4595,16 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="F3" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="H3" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -4612,13 +4618,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="F4" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -4632,13 +4638,13 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="F5" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -4652,16 +4658,16 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="F6" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="H6" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -4675,10 +4681,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F7" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -4692,16 +4698,16 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F8" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="H8" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -4718,7 +4724,7 @@
         <v>96</v>
       </c>
       <c r="F9" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -4732,16 +4738,16 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F10" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="H10" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -4758,7 +4764,7 @@
         <v>96</v>
       </c>
       <c r="F11" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -4772,10 +4778,10 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F12" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -4789,10 +4795,10 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F13" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -4806,10 +4812,10 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="F14" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -4823,10 +4829,10 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F15" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -4840,16 +4846,16 @@
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="F16" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="H16" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -4863,10 +4869,10 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F17" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -4880,16 +4886,16 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F18" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="H18" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
   </sheetData>
@@ -5046,10 +5052,10 @@
   <dimension ref="A1:V360"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B115" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A128" sqref="A128"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5114,10 +5120,10 @@
         <v>554</v>
       </c>
       <c r="O1" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="P1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="Q1" s="13" t="s">
         <v>157</v>
@@ -5135,7 +5141,7 @@
         <v>618</v>
       </c>
       <c r="V1" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -5266,7 +5272,7 @@
         <v>2</v>
       </c>
       <c r="V6" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
@@ -6828,7 +6834,7 @@
         <v>2</v>
       </c>
       <c r="V74" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.3">
@@ -7465,7 +7471,7 @@
         <v>562</v>
       </c>
       <c r="T103" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="U103">
         <f t="shared" si="3"/>
@@ -7723,7 +7729,7 @@
         <v>2</v>
       </c>
       <c r="V114" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="115" spans="1:22" x14ac:dyDescent="0.3">
@@ -8355,10 +8361,10 @@
         <v>4.5</v>
       </c>
       <c r="R144" s="8" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="T144" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="U144">
         <f t="shared" si="5"/>
@@ -10013,7 +10019,7 @@
         <v>19</v>
       </c>
       <c r="R239" s="9" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="U239">
         <f t="shared" si="7"/>
@@ -10927,7 +10933,7 @@
     </row>
     <row r="296" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="H296">
         <v>0.1</v>
@@ -10940,7 +10946,7 @@
         <v>0.1</v>
       </c>
       <c r="R296" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="U296">
         <f t="shared" si="9"/>
@@ -11883,7 +11889,7 @@
         <v>3</v>
       </c>
       <c r="V347" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="348" spans="1:22" x14ac:dyDescent="0.3">
@@ -12005,7 +12011,7 @@
     </row>
     <row r="355" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A355" s="17" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="O355">
         <v>4.0999999999999996</v>
@@ -12019,49 +12025,49 @@
     </row>
     <row r="356" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="O356">
         <v>1.5</v>
       </c>
       <c r="R356" s="20" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="357" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="O357">
         <v>3.3</v>
       </c>
       <c r="R357" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="S357" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="T357" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="358" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="O358">
         <v>1.6</v>
       </c>
       <c r="R358" t="s">
+        <v>893</v>
+      </c>
+      <c r="S358" t="s">
         <v>894</v>
-      </c>
-      <c r="S358" t="s">
-        <v>895</v>
       </c>
     </row>
     <row r="359" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="G359">
         <v>5.5</v>
@@ -12070,10 +12076,10 @@
         <v>4.2</v>
       </c>
       <c r="R359" t="s">
+        <v>888</v>
+      </c>
+      <c r="S359" t="s">
         <v>889</v>
-      </c>
-      <c r="S359" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="360" spans="1:21" x14ac:dyDescent="0.3">
@@ -12090,7 +12096,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="R360" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
   </sheetData>
@@ -12137,7 +12143,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12151,130 +12157,133 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="D1" s="18" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>727</v>
+        <v>921</v>
+      </c>
+      <c r="C2" t="s">
+        <v>920</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>728</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>729</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>730</v>
-      </c>
       <c r="D4" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>735</v>
+      </c>
+      <c r="B10" t="s">
         <v>736</v>
-      </c>
-      <c r="B10" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>875</v>
+      </c>
+      <c r="B12" t="s">
+        <v>877</v>
+      </c>
+      <c r="C12" t="s">
         <v>876</v>
-      </c>
-      <c r="B12" t="s">
-        <v>878</v>
-      </c>
-      <c r="C12" t="s">
-        <v>877</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>916</v>
+      </c>
+      <c r="C13" t="s">
         <v>917</v>
-      </c>
-      <c r="C13" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
   </sheetData>
@@ -12301,16 +12310,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B1">
         <v>1000</v>
       </c>
       <c r="C1" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -12321,10 +12330,10 @@
         <v>700</v>
       </c>
       <c r="C2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D2" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated email campaign state
</commit_message>
<xml_diff>
--- a/Marketing planning.xlsx
+++ b/Marketing planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wstoop\Documents\thesapling-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563F05B1-219C-49FD-8C8F-D88972F2F84E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86D474A-231B-4395-BC58-B8B62F5BEEC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="961">
   <si>
     <t>Week</t>
   </si>
@@ -2942,6 +2942,15 @@
   </si>
   <si>
     <t>zat per ongeluk ook al bij de decembergroep</t>
+  </si>
+  <si>
+    <t>Sent flower update email</t>
+  </si>
+  <si>
+    <t>Chase</t>
+  </si>
+  <si>
+    <t>Toch gereageerd</t>
   </si>
 </sst>
 </file>
@@ -4634,10 +4643,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4646,7 +4655,7 @@
     <col min="4" max="4" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>99</v>
       </c>
@@ -4671,8 +4680,11 @@
       <c r="H1" s="18" t="s">
         <v>756</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="18" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -4691,8 +4703,11 @@
       <c r="G2" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -4714,8 +4729,11 @@
       <c r="H3" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -4734,8 +4752,11 @@
       <c r="G4" s="19" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -4754,8 +4775,11 @@
       <c r="G5" s="19" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -4777,8 +4801,11 @@
       <c r="H6" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -4795,7 +4822,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -4817,8 +4844,11 @@
       <c r="H8" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>97</v>
       </c>
@@ -4835,7 +4865,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -4857,8 +4887,11 @@
       <c r="H10" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -4875,7 +4908,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -4892,7 +4925,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>90</v>
       </c>
@@ -4909,7 +4942,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -4926,7 +4959,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>92</v>
       </c>
@@ -4943,7 +4976,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -4965,8 +4998,11 @@
       <c r="H16" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>98</v>
       </c>
@@ -4983,7 +5019,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>327</v>
       </c>
@@ -5004,6 +5040,9 @@
       </c>
       <c r="H18" t="s">
         <v>762</v>
+      </c>
+      <c r="I18" t="s">
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -5019,10 +5058,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5189,15 +5228,21 @@
         <v>937</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>337</v>
       </c>
+      <c r="B17" t="s">
+        <v>959</v>
+      </c>
       <c r="C17" t="s">
         <v>938</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>338</v>
       </c>
@@ -5205,7 +5250,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>339</v>
       </c>
@@ -5213,7 +5258,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>282</v>
       </c>
@@ -5224,7 +5269,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>340</v>
       </c>
@@ -5232,7 +5277,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>341</v>
       </c>
@@ -5240,7 +5285,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>342</v>
       </c>
@@ -5251,7 +5296,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>343</v>
       </c>
@@ -5259,7 +5304,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>344</v>
       </c>

</xml_diff>

<commit_message>
Found unseen youtube videos
</commit_message>
<xml_diff>
--- a/Marketing planning.xlsx
+++ b/Marketing planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wstoop\Documents\thesapling-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86D474A-231B-4395-BC58-B8B62F5BEEC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D50BB85-3189-4A28-AEBC-256F2172B4C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overzicht" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="964">
   <si>
     <t>Week</t>
   </si>
@@ -2952,12 +2952,21 @@
   <si>
     <t>Toch gereageerd</t>
   </si>
+  <si>
+    <t>LarssonLand</t>
+  </si>
+  <si>
+    <t>GEMIST!</t>
+  </si>
+  <si>
+    <t>ШоуМяу</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3036,6 +3045,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF030303"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -3070,7 +3085,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3110,6 +3125,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4643,10 +4659,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5043,6 +5059,22 @@
       </c>
       <c r="I18" t="s">
         <v>491</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>961</v>
+      </c>
+      <c r="D20" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
+        <v>963</v>
+      </c>
+      <c r="D21" t="s">
+        <v>962</v>
       </c>
     </row>
   </sheetData>
@@ -5060,7 +5092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Collected more outshouter data
</commit_message>
<xml_diff>
--- a/Marketing planning.xlsx
+++ b/Marketing planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wstoop\Documents\thesapling-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373D8B78-BE1A-4F9D-AB2D-7F417BBA54B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AF9EEA-1DBC-47D8-BE79-DFDCFBCC33F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="782" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overzicht" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="985">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="988">
   <si>
     <t>Week</t>
   </si>
@@ -2986,9 +2986,6 @@
     <t>j.borg@keele.ac.uk</t>
   </si>
   <si>
-    <t>Chakovsky</t>
-  </si>
-  <si>
     <t>mwiser@msu.edu</t>
   </si>
   <si>
@@ -3023,6 +3020,18 @@
   </si>
   <si>
     <t>ziek</t>
+  </si>
+  <si>
+    <t>albert.chak@gmail.com</t>
+  </si>
+  <si>
+    <t>Chan</t>
+  </si>
+  <si>
+    <t>lsoros@cs.ucf.edu; lsoros@nyu.edu</t>
+  </si>
+  <si>
+    <t>contact@eatcreatesleep.net</t>
   </si>
 </sst>
 </file>
@@ -5421,14 +5430,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:W360"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J102" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V119" sqref="V119"/>
+      <selection pane="bottomRight" activeCell="V50" sqref="V50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5512,13 +5520,13 @@
         <v>445</v>
       </c>
       <c r="U1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="V1" t="s">
         <v>900</v>
       </c>
       <c r="W1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
@@ -6111,7 +6119,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>348</v>
       </c>
@@ -6135,7 +6143,7 @@
         <v>1</v>
       </c>
       <c r="V33" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="W33" t="s">
         <v>751</v>
@@ -6489,6 +6497,9 @@
       <c r="U50">
         <v>1</v>
       </c>
+      <c r="V50" t="s">
+        <v>903</v>
+      </c>
       <c r="W50" t="s">
         <v>753</v>
       </c>
@@ -6889,7 +6900,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="74" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>680</v>
       </c>
@@ -7243,7 +7254,7 @@
         <v>648</v>
       </c>
       <c r="S93" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="U93">
         <v>1</v>
@@ -7446,7 +7457,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="104" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>294</v>
       </c>
@@ -7473,7 +7484,7 @@
         <v>1</v>
       </c>
       <c r="V104" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="W104" t="s">
         <v>753</v>
@@ -7512,7 +7523,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="107" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>236</v>
       </c>
@@ -7532,7 +7543,7 @@
         <v>1</v>
       </c>
       <c r="V107" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="W107" t="s">
         <v>751</v>
@@ -7648,7 +7659,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="114" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>886</v>
       </c>
@@ -7755,7 +7766,7 @@
         <v>1</v>
       </c>
       <c r="V118" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="W118" t="s">
         <v>753</v>
@@ -7969,7 +7980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>708</v>
       </c>
@@ -8162,7 +8173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>649</v>
       </c>
@@ -8186,7 +8197,7 @@
         <v>1</v>
       </c>
       <c r="V139" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="W139" t="s">
         <v>753</v>
@@ -8612,7 +8623,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="164" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>353</v>
       </c>
@@ -8636,7 +8647,7 @@
         <v>1</v>
       </c>
       <c r="V164" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="W164" t="s">
         <v>753</v>
@@ -8866,7 +8877,7 @@
         <v>575</v>
       </c>
       <c r="T176" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="U176">
         <v>2</v>
@@ -11392,11 +11403,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W360" xr:uid="{55BDA2F9-72C3-42C1-8CD7-73DE1DD64440}">
-    <filterColumn colId="21">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:W360" xr:uid="{55BDA2F9-72C3-42C1-8CD7-73DE1DD64440}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T308">
     <sortCondition descending="1" ref="Q2:Q308"/>
   </sortState>
@@ -11434,8 +11441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11490,6 +11497,9 @@
       <c r="A7" t="s">
         <v>731</v>
       </c>
+      <c r="B7" s="7" t="s">
+        <v>987</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -11582,7 +11592,7 @@
         <v>908</v>
       </c>
       <c r="B19" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C19" t="s">
         <v>969</v>
@@ -11592,27 +11602,33 @@
       <c r="A20" t="s">
         <v>909</v>
       </c>
+      <c r="B20" t="s">
+        <v>984</v>
+      </c>
       <c r="C20" t="s">
-        <v>972</v>
+        <v>985</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>910</v>
       </c>
-      <c r="B21" t="s">
-        <v>975</v>
+      <c r="B21" s="7" t="s">
+        <v>974</v>
       </c>
       <c r="C21" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>911</v>
       </c>
+      <c r="B22" t="s">
+        <v>986</v>
+      </c>
       <c r="C22" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -11620,7 +11636,7 @@
         <v>916</v>
       </c>
       <c r="B23" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C23" t="s">
         <v>970</v>
@@ -11630,9 +11646,11 @@
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
     <hyperlink ref="B15" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="B21" r:id="rId3" xr:uid="{7B064C93-8D3B-49D5-A6A0-C0BC717AB90C}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{90A95F1F-6950-4AFC-BE7E-97149B3CF303}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>